<commit_message>
Added productivity target inputs to Scneario. Functions with productivity dataframes. Added Radar chart for productivity targets Calculations for CO2 emitted, mitigated and net
Played around with pba analysis
</commit_message>
<xml_diff>
--- a/Current_Financial_Model.xlsx
+++ b/Current_Financial_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Francis/PycharmProjects/VerticalFarming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD9A1A6-FEFE-AD4F-A899-9D1FD01FE006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4340A06-5EBB-D846-9BC9-C0A1A36C3932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27220" yWindow="-1300" windowWidth="36780" windowHeight="18320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="21360" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="14" r:id="rId1"/>
@@ -1925,7 +1925,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="881">
   <si>
     <t>Packaging types &amp; ROUGH Cost per package</t>
   </si>
@@ -4538,6 +4538,36 @@
   </si>
   <si>
     <t>capex_full</t>
+  </si>
+  <si>
+    <t>target_productivity_space</t>
+  </si>
+  <si>
+    <t>target_productivity_energy</t>
+  </si>
+  <si>
+    <t>target_productivity_labour</t>
+  </si>
+  <si>
+    <t>target_productivity_water</t>
+  </si>
+  <si>
+    <t>target_productivity_nutrients</t>
+  </si>
+  <si>
+    <t>target_productivity_volume</t>
+  </si>
+  <si>
+    <t>target_productivity_CO2_net</t>
+  </si>
+  <si>
+    <t>target_productivity_plants</t>
+  </si>
+  <si>
+    <t>target_productivity_CO2_emit</t>
+  </si>
+  <si>
+    <t>target_productivity_CO2_miti</t>
   </si>
 </sst>
 </file>
@@ -5871,6 +5901,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5932,7 +5963,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -6156,28 +6186,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -6286,28 +6316,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -6407,28 +6437,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -6537,28 +6567,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -6658,28 +6688,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -6788,28 +6818,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -6909,28 +6939,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -7039,28 +7069,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-7.9453467335346917E-2</c:v>
+                  <c:v>-0.24285589089229545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.207800140113324E-3</c:v>
+                  <c:v>-4.9592599494643438E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8373334738601595E-2</c:v>
+                  <c:v>-3.4427064896155164E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9273562731264559E-2</c:v>
+                  <c:v>-2.3526836903492204E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9320729402763217E-2</c:v>
+                  <c:v>-1.3479670231993545E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8514834753096397E-2</c:v>
+                  <c:v>0.12341122369054316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7045447964745817E-2</c:v>
+                  <c:v>0.13194183690219261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2922092621660305E-2</c:v>
+                  <c:v>0.13781848155910709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.14331598785105873</c:v>
@@ -7450,28 +7480,28 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-17726.674835327263</c:v>
+                  <c:v>-54183.002379510188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>715.6846885045743</c:v>
+                  <c:v>-11064.487365538342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4099.231178636277</c:v>
+                  <c:v>-7680.940875406639</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6531.1552184183311</c:v>
+                  <c:v>-5249.0168356245849</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8772.7547681306241</c:v>
+                  <c:v>-3007.4172859122918</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10824.029827772894</c:v>
+                  <c:v>27533.985699562461</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12727.274728471926</c:v>
+                  <c:v>29437.230600261497</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14038.398993398023</c:v>
+                  <c:v>30748.354865187594</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>31974.890467860259</c:v>
@@ -7580,28 +7610,28 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-17726.674835327263</c:v>
+                  <c:v>-54183.002379510188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>715.6846885045743</c:v>
+                  <c:v>-11064.487365538342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4099.231178636277</c:v>
+                  <c:v>-7680.940875406639</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6531.1552184183311</c:v>
+                  <c:v>-5249.0168356245849</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8772.7547681306241</c:v>
+                  <c:v>-3007.4172859122918</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10824.029827772894</c:v>
+                  <c:v>27533.985699562461</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12727.274728471926</c:v>
+                  <c:v>29437.230600261497</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14038.398993398023</c:v>
+                  <c:v>30748.354865187594</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>31974.890467860259</c:v>
@@ -8410,28 +8440,28 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-17726.674835327263</c:v>
+                  <c:v>-54183.002379510188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>715.6846885045743</c:v>
+                  <c:v>-11064.487365538342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4099.231178636277</c:v>
+                  <c:v>-7680.940875406639</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6531.1552184183311</c:v>
+                  <c:v>-5249.0168356245849</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8772.7547681306241</c:v>
+                  <c:v>-3007.4172859122918</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10824.029827772894</c:v>
+                  <c:v>27533.985699562461</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12727.274728471926</c:v>
+                  <c:v>29437.230600261497</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14038.398993398023</c:v>
+                  <c:v>30748.354865187594</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>31974.890467860259</c:v>
@@ -8620,7 +8650,7 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>39967.780947032166</c:v>
+                  <c:v>64643.936437172168</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>96630.077384056305</c:v>
@@ -8690,7 +8720,7 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>9129.4651929772517</c:v>
+                  <c:v>-15546.69029716275</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>37718.008873324041</c:v>
@@ -11453,7 +11483,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.65184201819348098</c:v>
+                  <c:v>0.82818050488328576</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.51366499546627742</c:v>
@@ -11477,7 +11507,7 @@
                   <c:v>0.9022472241454822</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.3185344886939368</c:v>
+                  <c:v>-1.2741379547757472</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.0097648469642859</c:v>
@@ -14187,10 +14217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1FB0-CD2F-E14E-8300-C92D3DA9F93F}">
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A93" zoomScale="96" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -14507,7 +14537,7 @@
       </c>
       <c r="B35" s="342">
         <f>loan_interest</f>
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -14516,7 +14546,7 @@
       </c>
       <c r="B36" s="344">
         <f>loan_tenure</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -15255,6 +15285,96 @@
       <c r="B118" s="106">
         <f>'CapEx Breakdown'!D16+'CapEx Breakdown'!D17+'CapEx Breakdown'!D18+'CapEx Breakdown'!C18+'CapEx Breakdown'!C17+'CapEx Breakdown'!C16</f>
         <v>11000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="47" t="s">
+        <v>871</v>
+      </c>
+      <c r="B119">
+        <f>target_productivity_space</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="47" t="s">
+        <v>872</v>
+      </c>
+      <c r="B120">
+        <f>target_productivity_energy</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="47" t="s">
+        <v>873</v>
+      </c>
+      <c r="B121">
+        <f>target_productivity_labour</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="47" t="s">
+        <v>874</v>
+      </c>
+      <c r="B122">
+        <f>target_productivity_water</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="47" t="s">
+        <v>875</v>
+      </c>
+      <c r="B123">
+        <f>target_productivity_nutrients</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="47" t="s">
+        <v>876</v>
+      </c>
+      <c r="B124">
+        <f>target_productivity_volume</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="B125">
+        <f>target_productivity_plants</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="47" t="s">
+        <v>879</v>
+      </c>
+      <c r="B126">
+        <f>target_productivity_CO2</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="47" t="s">
+        <v>880</v>
+      </c>
+      <c r="B127">
+        <f>target_productivity_CO2_omitted</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="47" t="s">
+        <v>877</v>
+      </c>
+      <c r="B128">
+        <f>target_productivity_CO2_net</f>
+        <v>-100</v>
       </c>
     </row>
   </sheetData>
@@ -15270,6 +15390,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -15282,7 +15403,7 @@
   <dimension ref="A1:AA1007"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -15565,11 +15686,11 @@
       </c>
       <c r="C7" s="49">
         <f>Overview!F90</f>
-        <v>3330.6484122526804</v>
+        <v>5386.9947030976809</v>
       </c>
       <c r="D7" s="49">
         <f>Overview!H90</f>
-        <v>39967.780947032166</v>
+        <v>64643.936437172168</v>
       </c>
       <c r="E7" s="49">
         <f>Overview!I90</f>
@@ -15644,11 +15765,11 @@
       </c>
       <c r="C8" s="50">
         <f>Overview!F92</f>
-        <v>7028.2887660814413</v>
+        <v>4971.9424752364403</v>
       </c>
       <c r="D8" s="50">
         <f>Overview!H92</f>
-        <v>84339.465192977252</v>
+        <v>59663.30970283725</v>
       </c>
       <c r="E8" s="50">
         <f>Overview!I92</f>
@@ -15860,11 +15981,11 @@
       </c>
       <c r="C12" s="50">
         <f>Overview!F102</f>
-        <v>760.78876608144128</v>
+        <v>-1295.5575247635597</v>
       </c>
       <c r="D12" s="50">
         <f>Overview!H102</f>
-        <v>9129.4651929772517</v>
+        <v>-15546.69029716275</v>
       </c>
       <c r="E12" s="50">
         <f>Overview!I102</f>
@@ -15969,35 +16090,35 @@
       <c r="C14" s="78"/>
       <c r="D14" s="78">
         <f>Overview!H104</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="E14" s="78">
         <f>Overview!I104</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="F14" s="78">
         <f>Overview!J104</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="G14" s="78">
         <f>Overview!K104</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="H14" s="78">
         <f>Overview!L104</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="I14" s="78">
         <f>Overview!M104</f>
-        <v>16709.955871789567</v>
+        <v>0</v>
       </c>
       <c r="J14" s="78">
         <f>Overview!N104</f>
-        <v>16709.955871789567</v>
+        <v>0</v>
       </c>
       <c r="K14" s="78">
         <f>Overview!O104</f>
-        <v>16709.955871789567</v>
+        <v>0</v>
       </c>
       <c r="L14" s="78">
         <f>Overview!P104</f>
@@ -16047,63 +16168,63 @@
       <c r="C15" s="81"/>
       <c r="D15" s="78">
         <f>Overview!H105</f>
-        <v>-96690.044128210429</v>
+        <v>-90309.872074167521</v>
       </c>
       <c r="E15" s="78">
         <f>Overview!I105</f>
-        <v>-84814.590462831373</v>
+        <v>-70850.731355751792</v>
       </c>
       <c r="F15" s="78">
         <f>Overview!J105</f>
-        <v>-72345.364114183365</v>
+        <v>-49445.67656549449</v>
       </c>
       <c r="G15" s="78">
         <f>Overview!K105</f>
-        <v>-59252.67644810296</v>
+        <v>-25900.116296211458</v>
       </c>
       <c r="H15" s="78">
         <f>Overview!L105</f>
-        <v>-45505.354398718548</v>
+        <v>-1.2050804798491299E-10</v>
       </c>
       <c r="I15" s="78">
         <f>Overview!M105</f>
-        <v>-31070.666246864908</v>
+        <v>-1.3255885278340429E-10</v>
       </c>
       <c r="J15" s="78">
         <f>Overview!N105</f>
-        <v>-15914.243687418588</v>
+        <v>-1.4581473806174471E-10</v>
       </c>
       <c r="K15" s="78">
         <f>Overview!O105</f>
-        <v>4.9794834922067821E-11</v>
+        <v>-1.6039621186791918E-10</v>
       </c>
       <c r="L15" s="78">
         <f>Overview!P105</f>
-        <v>5.2284576668171209E-11</v>
+        <v>-1.764358330547111E-10</v>
       </c>
       <c r="M15" s="78">
         <f>Overview!Q105</f>
-        <v>5.4898805501579771E-11</v>
+        <v>-1.9407941636018222E-10</v>
       </c>
       <c r="N15" s="78">
         <f>Overview!R105</f>
-        <v>5.7643745776658758E-11</v>
+        <v>-2.1348735799620044E-10</v>
       </c>
       <c r="O15" s="78">
         <f>Overview!S105</f>
-        <v>6.0525933065491697E-11</v>
+        <v>-2.3483609379582046E-10</v>
       </c>
       <c r="P15" s="78">
         <f>Overview!T105</f>
-        <v>6.355222971876628E-11</v>
+        <v>-2.5831970317540249E-10</v>
       </c>
       <c r="Q15" s="78">
         <f>Overview!U105</f>
-        <v>6.67298412047046E-11</v>
+        <v>-2.8415167349294275E-10</v>
       </c>
       <c r="R15" s="78">
         <f>Overview!V105</f>
-        <v>7.006633326493983E-11</v>
+        <v>-3.1256684084223703E-10</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -16225,39 +16346,39 @@
       </c>
       <c r="C18" s="78">
         <f>C12-C16</f>
-        <v>-84.726580294804535</v>
+        <v>-2141.0728711398056</v>
       </c>
       <c r="D18" s="78">
         <f>D12-(D12*Overview!$B$54)-D14-D16</f>
-        <v>-17726.674835327263</v>
+        <v>-54183.002379510188</v>
       </c>
       <c r="E18" s="78">
         <f>E12-(E12*Overview!$B$54)-E14-E16</f>
-        <v>715.6846885045743</v>
+        <v>-11064.487365538342</v>
       </c>
       <c r="F18" s="78">
         <f>F12-(F12*Overview!$B$54)-F14-F16</f>
-        <v>4099.231178636277</v>
+        <v>-7680.940875406639</v>
       </c>
       <c r="G18" s="78">
         <f>G12-(G12*Overview!$B$54)-G14-G16</f>
-        <v>6531.1552184183311</v>
+        <v>-5249.0168356245849</v>
       </c>
       <c r="H18" s="78">
         <f>H12-(H12*Overview!$B$54)-H14-H16</f>
-        <v>8772.7547681306241</v>
+        <v>-3007.4172859122918</v>
       </c>
       <c r="I18" s="78">
         <f>I12-(I12*Overview!$B$54)-I14-I16</f>
-        <v>10824.029827772894</v>
+        <v>27533.985699562461</v>
       </c>
       <c r="J18" s="78">
         <f>J12-(J12*Overview!$B$54)-J14-J16</f>
-        <v>12727.274728471926</v>
+        <v>29437.230600261497</v>
       </c>
       <c r="K18" s="78">
         <f>K12-(K12*Overview!$B$54)-K14-K16</f>
-        <v>14038.398993398023</v>
+        <v>30748.354865187594</v>
       </c>
       <c r="L18" s="78">
         <f>L12-(L12*Overview!$B$54)-L14-L16</f>
@@ -16305,63 +16426,63 @@
       <c r="C19" s="51"/>
       <c r="D19" s="51">
         <f>-H3+D12</f>
-        <v>-213978.16534640256</v>
+        <v>-238654.32083654255</v>
       </c>
       <c r="E19" s="51">
         <f>D19+E12</f>
-        <v>-176260.15647307853</v>
+        <v>-200936.3119632185</v>
       </c>
       <c r="F19" s="51">
         <f>E19+F12</f>
-        <v>-135158.6011096228</v>
+        <v>-159834.75659976277</v>
       </c>
       <c r="G19" s="51">
         <f t="shared" ref="G19:J19" si="0">F19+G12</f>
-        <v>-91625.121706385005</v>
+        <v>-116301.27719652497</v>
       </c>
       <c r="H19" s="51">
         <f>G19+H12</f>
-        <v>-45850.042753434915</v>
+        <v>-70526.19824357488</v>
       </c>
       <c r="I19" s="51">
         <f t="shared" si="0"/>
-        <v>1976.3112591574463</v>
+        <v>-22699.844230982519</v>
       </c>
       <c r="J19" s="51">
         <f t="shared" si="0"/>
-        <v>51705.910172448843</v>
+        <v>27029.754682308878</v>
       </c>
       <c r="K19" s="51">
         <f t="shared" ref="K19:R19" si="1">J19+K12</f>
-        <v>102746.63335066634</v>
+        <v>78070.477860526371</v>
       </c>
       <c r="L19" s="51">
         <f t="shared" si="1"/>
-        <v>155013.89213155649</v>
+        <v>130337.73664141653</v>
       </c>
       <c r="M19" s="51">
         <f t="shared" si="1"/>
-        <v>208444.24501842947</v>
+        <v>183768.08952828951</v>
       </c>
       <c r="N19" s="51">
         <f t="shared" si="1"/>
-        <v>262953.10334903188</v>
+        <v>238276.94785889192</v>
       </c>
       <c r="O19" s="51">
         <f t="shared" si="1"/>
-        <v>318477.02562667377</v>
+        <v>293800.87013653381</v>
       </c>
       <c r="P19" s="51">
         <f t="shared" si="1"/>
-        <v>374973.71752022847</v>
+        <v>350297.56203008851</v>
       </c>
       <c r="Q19" s="51">
         <f t="shared" si="1"/>
-        <v>432379.73753300606</v>
+        <v>407703.5820428661</v>
       </c>
       <c r="R19" s="51">
         <f t="shared" si="1"/>
-        <v>490631.64416831656</v>
+        <v>465955.4886781766</v>
       </c>
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
@@ -16442,35 +16563,35 @@
       <c r="C21" s="15"/>
       <c r="D21" s="76">
         <f>(D18/$H$3)</f>
-        <v>-7.9453467335346917E-2</v>
+        <v>-0.24285589089229545</v>
       </c>
       <c r="E21" s="76">
         <f t="shared" ref="E21:R21" si="2">(E18/$H$3)</f>
-        <v>3.207800140113324E-3</v>
+        <v>-4.9592599494643438E-2</v>
       </c>
       <c r="F21" s="76">
         <f t="shared" si="2"/>
-        <v>1.8373334738601595E-2</v>
+        <v>-3.4427064896155164E-2</v>
       </c>
       <c r="G21" s="76">
         <f t="shared" si="2"/>
-        <v>2.9273562731264559E-2</v>
+        <v>-2.3526836903492204E-2</v>
       </c>
       <c r="H21" s="76">
         <f t="shared" si="2"/>
-        <v>3.9320729402763217E-2</v>
+        <v>-1.3479670231993545E-2</v>
       </c>
       <c r="I21" s="76">
         <f t="shared" si="2"/>
-        <v>4.8514834753096397E-2</v>
+        <v>0.12341122369054316</v>
       </c>
       <c r="J21" s="76">
         <f>(J18/$H$3)</f>
-        <v>5.7045447964745817E-2</v>
+        <v>0.13194183690219261</v>
       </c>
       <c r="K21" s="76">
         <f t="shared" si="2"/>
-        <v>6.2922092621660305E-2</v>
+        <v>0.13781848155910709</v>
       </c>
       <c r="L21" s="76">
         <f t="shared" si="2"/>
@@ -45136,8 +45257,8 @@
   </sheetPr>
   <dimension ref="A1:V156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="G37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -45156,26 +45277,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="13">
-      <c r="A1" s="365" t="s">
+      <c r="A1" s="366" t="s">
         <v>518</v>
       </c>
-      <c r="B1" s="366"/>
-      <c r="C1" s="366"/>
-      <c r="D1" s="366"/>
-      <c r="E1" s="366"/>
-      <c r="F1" s="366"/>
-      <c r="G1" s="366"/>
-      <c r="H1" s="366"/>
+      <c r="B1" s="367"/>
+      <c r="C1" s="367"/>
+      <c r="D1" s="367"/>
+      <c r="E1" s="367"/>
+      <c r="F1" s="367"/>
+      <c r="G1" s="367"/>
+      <c r="H1" s="367"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A2" s="366"/>
-      <c r="B2" s="366"/>
-      <c r="C2" s="366"/>
-      <c r="D2" s="366"/>
-      <c r="E2" s="366"/>
-      <c r="F2" s="366"/>
-      <c r="G2" s="366"/>
-      <c r="H2" s="366"/>
+      <c r="A2" s="367"/>
+      <c r="B2" s="367"/>
+      <c r="C2" s="367"/>
+      <c r="D2" s="367"/>
+      <c r="E2" s="367"/>
+      <c r="F2" s="367"/>
+      <c r="G2" s="367"/>
+      <c r="H2" s="367"/>
     </row>
     <row r="3" spans="1:22" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="59" t="s">
@@ -45183,28 +45304,28 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="13">
-      <c r="A4" s="367" t="s">
+      <c r="A4" s="368" t="s">
         <v>517</v>
       </c>
-      <c r="B4" s="366"/>
-      <c r="C4" s="366"/>
-      <c r="D4" s="366"/>
-      <c r="E4" s="366"/>
-      <c r="F4" s="366"/>
-      <c r="G4" s="366"/>
-      <c r="H4" s="366"/>
+      <c r="B4" s="367"/>
+      <c r="C4" s="367"/>
+      <c r="D4" s="367"/>
+      <c r="E4" s="367"/>
+      <c r="F4" s="367"/>
+      <c r="G4" s="367"/>
+      <c r="H4" s="367"/>
     </row>
     <row r="5" spans="1:22" ht="13">
-      <c r="A5" s="368" t="s">
+      <c r="A5" s="369" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="366"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
-      <c r="G5" s="366"/>
-      <c r="H5" s="366"/>
+      <c r="B5" s="367"/>
+      <c r="C5" s="367"/>
+      <c r="D5" s="367"/>
+      <c r="E5" s="367"/>
+      <c r="F5" s="367"/>
+      <c r="G5" s="367"/>
+      <c r="H5" s="367"/>
     </row>
     <row r="6" spans="1:22" s="26" customFormat="1" ht="13">
       <c r="A6" s="92" t="s">
@@ -45219,16 +45340,16 @@
       <c r="H6" s="93"/>
     </row>
     <row r="7" spans="1:22" ht="13">
-      <c r="A7" s="369" t="s">
+      <c r="A7" s="370" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="366"/>
-      <c r="C7" s="366"/>
-      <c r="D7" s="366"/>
-      <c r="E7" s="366"/>
-      <c r="F7" s="366"/>
-      <c r="G7" s="366"/>
-      <c r="H7" s="366"/>
+      <c r="B7" s="367"/>
+      <c r="C7" s="367"/>
+      <c r="D7" s="367"/>
+      <c r="E7" s="367"/>
+      <c r="F7" s="367"/>
+      <c r="G7" s="367"/>
+      <c r="H7" s="367"/>
     </row>
     <row r="8" spans="1:22" s="26" customFormat="1" ht="13">
       <c r="A8" s="256" t="s">
@@ -45292,8 +45413,8 @@
       <c r="Q13" s="218"/>
       <c r="R13" s="219"/>
       <c r="S13" s="219"/>
-      <c r="T13" s="364"/>
-      <c r="U13" s="364"/>
+      <c r="T13" s="365"/>
+      <c r="U13" s="365"/>
     </row>
     <row r="14" spans="1:22" ht="16">
       <c r="A14" s="2" t="s">
@@ -45478,7 +45599,7 @@
       </c>
       <c r="D18" s="269"/>
       <c r="E18" s="269"/>
-      <c r="F18" s="371" t="s">
+      <c r="F18" s="372" t="s">
         <v>618</v>
       </c>
       <c r="G18" s="323" t="s">
@@ -45529,7 +45650,7 @@
       </c>
       <c r="D19" s="269"/>
       <c r="E19" s="269"/>
-      <c r="F19" s="371"/>
+      <c r="F19" s="372"/>
       <c r="G19" s="292" t="s">
         <v>585</v>
       </c>
@@ -45676,7 +45797,7 @@
       </c>
       <c r="D23" s="269"/>
       <c r="E23" s="269"/>
-      <c r="F23" s="380" t="s">
+      <c r="F23" s="381" t="s">
         <v>316</v>
       </c>
       <c r="G23" s="326" t="s">
@@ -45708,7 +45829,7 @@
       </c>
       <c r="D24" s="269"/>
       <c r="E24" s="269"/>
-      <c r="F24" s="380"/>
+      <c r="F24" s="381"/>
       <c r="G24" s="326" t="s">
         <v>596</v>
       </c>
@@ -45740,7 +45861,7 @@
       </c>
       <c r="D25" s="269"/>
       <c r="E25" s="269"/>
-      <c r="F25" s="379" t="s">
+      <c r="F25" s="380" t="s">
         <v>542</v>
       </c>
       <c r="G25" s="323" t="s">
@@ -45781,7 +45902,7 @@
       </c>
       <c r="D26" s="269"/>
       <c r="E26" s="269"/>
-      <c r="F26" s="379"/>
+      <c r="F26" s="380"/>
       <c r="G26" s="323" t="s">
         <v>315</v>
       </c>
@@ -45810,7 +45931,7 @@
       <c r="A27" s="4"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
-      <c r="F27" s="377" t="s">
+      <c r="F27" s="378" t="s">
         <v>588</v>
       </c>
       <c r="G27" s="185" t="s">
@@ -45843,7 +45964,7 @@
       </c>
       <c r="B28" s="54"/>
       <c r="C28" s="47"/>
-      <c r="F28" s="378"/>
+      <c r="F28" s="379"/>
       <c r="G28" s="185" t="s">
         <v>315</v>
       </c>
@@ -45876,7 +45997,7 @@
         <v>79</v>
       </c>
       <c r="C29" s="47"/>
-      <c r="F29" s="381" t="s">
+      <c r="F29" s="382" t="s">
         <v>587</v>
       </c>
       <c r="G29" s="185" t="s">
@@ -45911,7 +46032,7 @@
         <v>865</v>
       </c>
       <c r="C30" s="170"/>
-      <c r="F30" s="378"/>
+      <c r="F30" s="379"/>
       <c r="G30" s="185" t="s">
         <v>483</v>
       </c>
@@ -45944,7 +46065,7 @@
         <v>165</v>
       </c>
       <c r="C31" s="170"/>
-      <c r="F31" s="373" t="s">
+      <c r="F31" s="374" t="s">
         <v>531</v>
       </c>
       <c r="G31" s="212" t="s">
@@ -45976,7 +46097,7 @@
         <v>164</v>
       </c>
       <c r="C32" s="170"/>
-      <c r="F32" s="374"/>
+      <c r="F32" s="375"/>
       <c r="G32" s="212" t="s">
         <v>315</v>
       </c>
@@ -46035,7 +46156,7 @@
       <c r="B34" s="356" t="s">
         <v>165</v>
       </c>
-      <c r="F34" s="370" t="s">
+      <c r="F34" s="371" t="s">
         <v>615</v>
       </c>
       <c r="G34" s="185" t="s">
@@ -46069,7 +46190,7 @@
       <c r="C35" s="254" t="s">
         <v>489</v>
       </c>
-      <c r="F35" s="370"/>
+      <c r="F35" s="371"/>
       <c r="G35" s="185" t="s">
         <v>533</v>
       </c>
@@ -46101,7 +46222,7 @@
       <c r="C36" s="264">
         <v>8</v>
       </c>
-      <c r="F36" s="370"/>
+      <c r="F36" s="371"/>
       <c r="G36" s="185" t="s">
         <v>534</v>
       </c>
@@ -46134,7 +46255,7 @@
         <f>C36*16</f>
         <v>128</v>
       </c>
-      <c r="F37" s="370"/>
+      <c r="F37" s="371"/>
       <c r="G37" s="185" t="s">
         <v>535</v>
       </c>
@@ -46165,7 +46286,7 @@
         <f>C36*VLOOKUP(B36, Database!A97:I107, 5, FALSE)</f>
         <v>2880</v>
       </c>
-      <c r="F38" s="370"/>
+      <c r="F38" s="371"/>
       <c r="G38" s="185" t="s">
         <v>536</v>
       </c>
@@ -46195,7 +46316,7 @@
         <v>507</v>
       </c>
       <c r="C39" s="170"/>
-      <c r="F39" s="375" t="s">
+      <c r="F39" s="376" t="s">
         <v>589</v>
       </c>
       <c r="G39" s="212" t="s">
@@ -46227,7 +46348,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="170"/>
-      <c r="F40" s="376"/>
+      <c r="F40" s="377"/>
       <c r="G40" s="212" t="s">
         <v>315</v>
       </c>
@@ -46261,7 +46382,7 @@
       </c>
       <c r="C41" s="170"/>
       <c r="D41" s="55"/>
-      <c r="F41" s="371" t="s">
+      <c r="F41" s="372" t="s">
         <v>613</v>
       </c>
       <c r="G41" s="292" t="s">
@@ -46292,7 +46413,7 @@
         <v>166</v>
       </c>
       <c r="C42" s="170"/>
-      <c r="F42" s="371"/>
+      <c r="F42" s="372"/>
       <c r="G42" s="212" t="s">
         <v>614</v>
       </c>
@@ -46330,11 +46451,11 @@
         <v>722</v>
       </c>
       <c r="C44" s="170"/>
-      <c r="G44" s="382" t="s">
+      <c r="G44" s="383" t="s">
         <v>602</v>
       </c>
-      <c r="H44" s="382"/>
-      <c r="I44" s="382"/>
+      <c r="H44" s="383"/>
+      <c r="I44" s="383"/>
     </row>
     <row r="45" spans="1:12" s="160" customFormat="1" ht="16">
       <c r="A45" s="171" t="s">
@@ -46383,15 +46504,15 @@
         <v>511</v>
       </c>
       <c r="I46" s="183">
-        <f>SUM(I68:I71)/B17</f>
-        <v>133.62761372966361</v>
+        <f>SUM(V68:V71)/growing_area_full</f>
+        <v>74.536245439495715</v>
       </c>
       <c r="J46" s="275">
-        <v>205</v>
+        <v>90</v>
       </c>
       <c r="K46" s="183">
         <f>I46/J46</f>
-        <v>0.65184201819348098</v>
+        <v>0.82818050488328576</v>
       </c>
       <c r="L46" s="269">
         <v>1</v>
@@ -46423,7 +46544,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K47" s="183">
-        <f t="shared" ref="K47:K55" si="2">I47/J47</f>
+        <f>I47/J47</f>
         <v>0.51366499546627742</v>
       </c>
       <c r="L47" s="269">
@@ -46456,7 +46577,7 @@
         <v>6</v>
       </c>
       <c r="K48" s="183">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K48:K55" si="2">I48/J48</f>
         <v>0.62050345962648679</v>
       </c>
       <c r="L48" s="269">
@@ -46643,11 +46764,11 @@
         <v>127.41379547757472</v>
       </c>
       <c r="J54" s="275">
-        <v>-400</v>
+        <v>-100</v>
       </c>
       <c r="K54" s="183">
         <f t="shared" si="2"/>
-        <v>-0.3185344886939368</v>
+        <v>-1.2741379547757472</v>
       </c>
       <c r="L54" s="269">
         <v>1</v>
@@ -46658,7 +46779,7 @@
         <v>210</v>
       </c>
       <c r="B55" s="248">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C55" s="48"/>
       <c r="D55" s="6"/>
@@ -46693,7 +46814,7 @@
         <v>212</v>
       </c>
       <c r="B56" s="249">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C56" s="48"/>
       <c r="D56" s="26"/>
@@ -46718,6 +46839,10 @@
       <c r="A58" s="26"/>
       <c r="B58" s="26"/>
       <c r="C58" s="54"/>
+      <c r="I58" s="102">
+        <f>SUM(V68:V71)</f>
+        <v>8854.9059582120917</v>
+      </c>
       <c r="J58" s="26"/>
     </row>
     <row r="59" spans="1:12" s="28" customFormat="1" ht="16">
@@ -48126,8 +48251,8 @@
       <c r="D86" s="206"/>
       <c r="E86" s="206"/>
       <c r="F86" s="35">
-        <f>(B$23*F68/0.2*4)/12</f>
-        <v>1028.1731454225001</v>
+        <f>(B$23*F68/crop1_product_weight)</f>
+        <v>3084.5194362675002</v>
       </c>
       <c r="G86" s="194">
         <f>I86/12</f>
@@ -48135,61 +48260,61 @@
       </c>
       <c r="H86" s="35">
         <f>F86*12</f>
-        <v>12338.077745070001</v>
+        <v>37014.233235210006</v>
       </c>
       <c r="I86" s="36">
         <f>C$23*(y2_wa_yield_crop1/H21)</f>
         <v>56723.198359905007</v>
       </c>
-      <c r="J86" s="387">
+      <c r="J86" s="364">
         <f>$C$23*(y3_wa_yield_crop1/$H$21)</f>
         <v>57803.51162470501</v>
       </c>
-      <c r="K86" s="387">
+      <c r="K86" s="364">
         <f>$C$23*(K68/$H$21)</f>
         <v>58579.986783779997</v>
       </c>
-      <c r="L86" s="387">
+      <c r="L86" s="364">
         <f t="shared" ref="L86:V86" si="11">$C$23*(L68/$H$21)</f>
         <v>59295.694321710005</v>
       </c>
-      <c r="M86" s="387">
+      <c r="M86" s="364">
         <f t="shared" si="11"/>
         <v>59950.634238494997</v>
       </c>
-      <c r="N86" s="387">
+      <c r="N86" s="364">
         <f t="shared" si="11"/>
         <v>60558.310449944998</v>
       </c>
-      <c r="O86" s="387">
+      <c r="O86" s="364">
         <f t="shared" si="11"/>
         <v>60976.931840055011</v>
       </c>
-      <c r="P86" s="387">
+      <c r="P86" s="364">
         <f t="shared" si="11"/>
         <v>61368.545398545</v>
       </c>
-      <c r="Q86" s="387">
+      <c r="Q86" s="364">
         <f t="shared" si="11"/>
         <v>61739.903083320009</v>
       </c>
-      <c r="R86" s="387">
+      <c r="R86" s="364">
         <f t="shared" si="11"/>
         <v>62084.252936475008</v>
       </c>
-      <c r="S86" s="387">
+      <c r="S86" s="364">
         <f t="shared" si="11"/>
         <v>62408.346915915005</v>
       </c>
-      <c r="T86" s="387">
+      <c r="T86" s="364">
         <f t="shared" si="11"/>
         <v>62718.936979545004</v>
       </c>
-      <c r="U86" s="387">
+      <c r="U86" s="364">
         <f t="shared" si="11"/>
         <v>63009.27116946</v>
       </c>
-      <c r="V86" s="387">
+      <c r="V86" s="364">
         <f t="shared" si="11"/>
         <v>63279.349485660001</v>
       </c>
@@ -48441,7 +48566,7 @@
       <c r="E90" s="21"/>
       <c r="F90" s="38">
         <f>SUM(F84:F89)</f>
-        <v>3330.6484122526804</v>
+        <v>5386.9947030976809</v>
       </c>
       <c r="G90" s="195">
         <f>SUM(G84:G89)</f>
@@ -48449,7 +48574,7 @@
       </c>
       <c r="H90" s="38">
         <f t="shared" ref="H90:V90" si="12">SUM(H84:H89)</f>
-        <v>39967.780947032166</v>
+        <v>64643.936437172168</v>
       </c>
       <c r="I90" s="38">
         <f t="shared" si="12"/>
@@ -48542,7 +48667,7 @@
       <c r="E92" s="204"/>
       <c r="F92" s="83">
         <f>F81-F90</f>
-        <v>7028.2887660814413</v>
+        <v>4971.9424752364403</v>
       </c>
       <c r="G92" s="83">
         <f>G81-G90</f>
@@ -48550,7 +48675,7 @@
       </c>
       <c r="H92" s="83">
         <f>H81-H90</f>
-        <v>84339.465192977252</v>
+        <v>59663.30970283725</v>
       </c>
       <c r="I92" s="83">
         <f t="shared" ref="I92:V92" si="13">I81-I90</f>
@@ -49192,7 +49317,7 @@
       <c r="E102" s="204"/>
       <c r="F102" s="43">
         <f>F92-F100</f>
-        <v>760.78876608144128</v>
+        <v>-1295.5575247635597</v>
       </c>
       <c r="G102" s="43">
         <f>G92-G100</f>
@@ -49200,7 +49325,7 @@
       </c>
       <c r="H102" s="43">
         <f>H92-H100</f>
-        <v>9129.4651929772517</v>
+        <v>-15546.69029716275</v>
       </c>
       <c r="I102" s="43">
         <f>I92-I100</f>
@@ -49293,43 +49418,43 @@
       <c r="E104" s="206"/>
       <c r="F104" s="106">
         <f>H104/12</f>
-        <v>1392.4963226491307</v>
+        <v>2374.1773271527068</v>
       </c>
       <c r="G104" s="106">
         <f>I104/12</f>
-        <v>1392.4963226491307</v>
+        <v>2374.1773271527068</v>
       </c>
       <c r="H104" s="78">
         <f>IF($B$56/H73&gt;=1,  (Overview!$B$55*Overview!$B$53)/(1-(1+Overview!$B$55)^(-Overview!$B$56)), 0)</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="I104" s="78">
         <f>IF($B$56/I73&gt;=1, H104, 0)</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="J104" s="78">
         <f>IF($B$56/J73&gt;=1, I104, 0)</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="K104" s="78">
         <f t="shared" ref="K104:V104" si="19">IF($B$56/K73&gt;=1, J104, 0)</f>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="L104" s="78">
         <f t="shared" si="19"/>
-        <v>16709.955871789567</v>
+        <v>28490.127925832483</v>
       </c>
       <c r="M104" s="78">
         <f t="shared" si="19"/>
-        <v>16709.955871789567</v>
+        <v>0</v>
       </c>
       <c r="N104" s="78">
         <f t="shared" si="19"/>
-        <v>16709.955871789567</v>
+        <v>0</v>
       </c>
       <c r="O104" s="78">
         <f t="shared" si="19"/>
-        <v>16709.955871789567</v>
+        <v>0</v>
       </c>
       <c r="P104" s="78">
         <f t="shared" si="19"/>
@@ -49374,67 +49499,67 @@
       </c>
       <c r="G105" s="196">
         <f>H105</f>
-        <v>-96690.044128210429</v>
+        <v>-90309.872074167521</v>
       </c>
       <c r="H105" s="81">
         <f>F105+H104+(F105*$B$55)</f>
-        <v>-96690.044128210429</v>
+        <v>-90309.872074167521</v>
       </c>
       <c r="I105" s="81">
         <f t="shared" ref="I105:V105" si="20">H105+I104+(H105*$B$55)</f>
-        <v>-84814.590462831373</v>
+        <v>-70850.731355751792</v>
       </c>
       <c r="J105" s="81">
         <f>I105+J104+(I105*$B$55)</f>
-        <v>-72345.364114183365</v>
+        <v>-49445.67656549449</v>
       </c>
       <c r="K105" s="81">
         <f t="shared" si="20"/>
-        <v>-59252.67644810296</v>
+        <v>-25900.116296211458</v>
       </c>
       <c r="L105" s="81">
         <f t="shared" si="20"/>
-        <v>-45505.354398718548</v>
+        <v>-1.2050804798491299E-10</v>
       </c>
       <c r="M105" s="81">
         <f t="shared" si="20"/>
-        <v>-31070.666246864908</v>
+        <v>-1.3255885278340429E-10</v>
       </c>
       <c r="N105" s="81">
         <f t="shared" si="20"/>
-        <v>-15914.243687418588</v>
+        <v>-1.4581473806174471E-10</v>
       </c>
       <c r="O105" s="81">
         <f t="shared" si="20"/>
-        <v>4.9794834922067821E-11</v>
+        <v>-1.6039621186791918E-10</v>
       </c>
       <c r="P105" s="81">
         <f t="shared" si="20"/>
-        <v>5.2284576668171209E-11</v>
+        <v>-1.764358330547111E-10</v>
       </c>
       <c r="Q105" s="81">
         <f t="shared" si="20"/>
-        <v>5.4898805501579771E-11</v>
+        <v>-1.9407941636018222E-10</v>
       </c>
       <c r="R105" s="81">
         <f t="shared" si="20"/>
-        <v>5.7643745776658758E-11</v>
+        <v>-2.1348735799620044E-10</v>
       </c>
       <c r="S105" s="81">
         <f t="shared" si="20"/>
-        <v>6.0525933065491697E-11</v>
+        <v>-2.3483609379582046E-10</v>
       </c>
       <c r="T105" s="81">
         <f t="shared" si="20"/>
-        <v>6.355222971876628E-11</v>
+        <v>-2.5831970317540249E-10</v>
       </c>
       <c r="U105" s="81">
         <f t="shared" si="20"/>
-        <v>6.67298412047046E-11</v>
+        <v>-2.8415167349294275E-10</v>
       </c>
       <c r="V105" s="81">
         <f t="shared" si="20"/>
-        <v>7.006633326493983E-11</v>
+        <v>-3.1256684084223703E-10</v>
       </c>
     </row>
     <row r="106" spans="1:22" ht="13">
@@ -49619,7 +49744,7 @@
       <c r="E109" s="206"/>
       <c r="F109" s="42">
         <f>F102</f>
-        <v>760.78876608144128</v>
+        <v>-1295.5575247635597</v>
       </c>
       <c r="G109" s="42">
         <f>G102</f>
@@ -49627,35 +49752,35 @@
       </c>
       <c r="H109" s="42">
         <f>H102-H106-H104-H107</f>
-        <v>-17726.674835327263</v>
+        <v>-54183.002379510188</v>
       </c>
       <c r="I109" s="42">
         <f t="shared" ref="I109:V109" si="22">I102-I106-I104-I107</f>
-        <v>715.6846885045743</v>
+        <v>-11064.487365538342</v>
       </c>
       <c r="J109" s="42">
         <f t="shared" si="22"/>
-        <v>4099.231178636277</v>
+        <v>-7680.940875406639</v>
       </c>
       <c r="K109" s="42">
         <f t="shared" si="22"/>
-        <v>6531.1552184183311</v>
+        <v>-5249.0168356245849</v>
       </c>
       <c r="L109" s="42">
         <f t="shared" si="22"/>
-        <v>8772.7547681306241</v>
+        <v>-3007.4172859122918</v>
       </c>
       <c r="M109" s="42">
         <f t="shared" si="22"/>
-        <v>10824.029827772894</v>
+        <v>27533.985699562461</v>
       </c>
       <c r="N109" s="42">
         <f t="shared" si="22"/>
-        <v>12727.274728471926</v>
+        <v>29437.230600261497</v>
       </c>
       <c r="O109" s="42">
         <f t="shared" si="22"/>
-        <v>14038.398993398023</v>
+        <v>30748.354865187594</v>
       </c>
       <c r="P109" s="42">
         <f t="shared" si="22"/>
@@ -50015,55 +50140,55 @@
         <v>0</v>
       </c>
       <c r="J116" s="82">
-        <f>I116*(1-labour_improvement)</f>
+        <f t="shared" ref="J116:V116" si="26">I116*(1-labour_improvement)</f>
         <v>0</v>
       </c>
       <c r="K116" s="82">
-        <f>J116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L116" s="82">
-        <f>K116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M116" s="82">
-        <f>L116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="N116" s="82">
-        <f>M116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O116" s="82">
-        <f>N116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="P116" s="82">
-        <f>O116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="Q116" s="82">
-        <f>P116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R116" s="82">
-        <f>Q116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="S116" s="82">
-        <f>R116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="T116" s="82">
-        <f>S116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="U116" s="82">
-        <f>T116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="V116" s="82">
-        <f>U116*(1-labour_improvement)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
     </row>
@@ -50084,47 +50209,47 @@
         <v>1500</v>
       </c>
       <c r="H117" s="38">
-        <f t="shared" ref="H117:R117" si="26">SUM(H113:H115)</f>
+        <f t="shared" ref="H117:R117" si="27">SUM(H113:H115)</f>
         <v>18000</v>
       </c>
       <c r="I117" s="46">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="J117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="K117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="L117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="M117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="N117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="O117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="P117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="Q117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="R117" s="84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18000</v>
       </c>
       <c r="S117" s="84">
@@ -50248,11 +50373,11 @@
         <v>102</v>
       </c>
       <c r="H120" s="35">
-        <f t="shared" ref="H120:I125" si="27">F130*$C120</f>
+        <f t="shared" ref="H120:I125" si="28">F130*$C120</f>
         <v>0</v>
       </c>
       <c r="I120" s="36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J120" s="82">
@@ -50260,51 +50385,51 @@
         <v>0</v>
       </c>
       <c r="K120" s="82">
-        <f t="shared" ref="K120:Q120" si="28">J120</f>
+        <f t="shared" ref="K120:Q120" si="29">J120</f>
         <v>0</v>
       </c>
       <c r="L120" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M120" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N120" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="O120" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P120" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="Q120" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R120" s="82">
-        <f t="shared" ref="R120:V126" si="29">Q120</f>
+        <f t="shared" ref="R120:V126" si="30">Q120</f>
         <v>0</v>
       </c>
       <c r="S120" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="T120" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="U120" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="V120" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -50316,7 +50441,7 @@
         <v>1560</v>
       </c>
       <c r="C121" s="35">
-        <f t="shared" ref="C121:C126" si="30">B121*12</f>
+        <f t="shared" ref="C121:C126" si="31">B121*12</f>
         <v>18720</v>
       </c>
       <c r="D121" s="35"/>
@@ -50328,63 +50453,63 @@
         <v>102</v>
       </c>
       <c r="H121" s="35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="I121" s="36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>18720</v>
       </c>
       <c r="J121" s="82">
-        <f t="shared" ref="J121:Q126" si="31">I121</f>
+        <f t="shared" ref="J121:Q126" si="32">I121</f>
         <v>18720</v>
       </c>
       <c r="K121" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="L121" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="M121" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="N121" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="O121" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="P121" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="Q121" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="R121" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="S121" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="T121" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="U121" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="V121" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
     </row>
@@ -50396,7 +50521,7 @@
         <v>2025</v>
       </c>
       <c r="C122" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>24300</v>
       </c>
       <c r="D122" s="35"/>
@@ -50408,63 +50533,63 @@
         <v>102</v>
       </c>
       <c r="H122" s="35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>12150</v>
       </c>
       <c r="I122" s="36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>12150</v>
       </c>
       <c r="J122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="K122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="L122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="M122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="N122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="O122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="P122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="Q122" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12150</v>
       </c>
       <c r="R122" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12150</v>
       </c>
       <c r="S122" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12150</v>
       </c>
       <c r="T122" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12150</v>
       </c>
       <c r="U122" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12150</v>
       </c>
       <c r="V122" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12150</v>
       </c>
     </row>
@@ -50488,63 +50613,63 @@
         <v>102</v>
       </c>
       <c r="H123" s="35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>24300</v>
       </c>
       <c r="I123" s="36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>24300</v>
       </c>
       <c r="J123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="K123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="L123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="M123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="N123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="O123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="P123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="Q123" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>24300</v>
       </c>
       <c r="R123" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>24300</v>
       </c>
       <c r="S123" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>24300</v>
       </c>
       <c r="T123" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>24300</v>
       </c>
       <c r="U123" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>24300</v>
       </c>
       <c r="V123" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>24300</v>
       </c>
     </row>
@@ -50556,7 +50681,7 @@
         <v>1560</v>
       </c>
       <c r="C124" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>18720</v>
       </c>
       <c r="D124" s="35"/>
@@ -50568,63 +50693,63 @@
         <v>102</v>
       </c>
       <c r="H124" s="35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="I124" s="36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>18720</v>
       </c>
       <c r="J124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="K124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="L124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="M124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="N124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="O124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="P124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="Q124" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18720</v>
       </c>
       <c r="R124" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="S124" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="T124" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="U124" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
       <c r="V124" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>18720</v>
       </c>
     </row>
@@ -50636,7 +50761,7 @@
         <v>2025</v>
       </c>
       <c r="C125" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>24300</v>
       </c>
       <c r="D125" s="35"/>
@@ -50648,7 +50773,7 @@
         <v>102</v>
       </c>
       <c r="H125" s="35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>24300</v>
       </c>
       <c r="I125" s="36">
@@ -50660,51 +50785,51 @@
         <v>0</v>
       </c>
       <c r="K125" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="L125" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M125" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N125" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O125" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P125" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q125" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R125" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="S125" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="T125" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="U125" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="V125" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -50716,7 +50841,7 @@
         <v>624</v>
       </c>
       <c r="C126" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>7488</v>
       </c>
       <c r="D126" s="35"/>
@@ -50736,55 +50861,55 @@
         <v>7488</v>
       </c>
       <c r="J126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="K126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="L126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="M126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="N126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="O126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="P126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="Q126" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7488</v>
       </c>
       <c r="R126" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7488</v>
       </c>
       <c r="S126" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7488</v>
       </c>
       <c r="T126" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7488</v>
       </c>
       <c r="U126" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7488</v>
       </c>
       <c r="V126" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7488</v>
       </c>
     </row>
@@ -50805,63 +50930,63 @@
         <v>6781.5</v>
       </c>
       <c r="H127" s="38">
-        <f t="shared" ref="H127:V127" si="32">SUM(H120:H126)</f>
+        <f t="shared" ref="H127:V127" si="33">SUM(H120:H126)</f>
         <v>60750</v>
       </c>
       <c r="I127" s="46">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="J127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="K127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="L127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="M127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="N127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="O127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="P127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="Q127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="R127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="S127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="T127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="U127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
       <c r="V127" s="84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>81378</v>
       </c>
     </row>
@@ -50964,51 +51089,51 @@
         <v>0</v>
       </c>
       <c r="I130" s="206">
-        <f t="shared" ref="I130:O130" si="33">H130</f>
+        <f t="shared" ref="I130:O130" si="34">H130</f>
         <v>0</v>
       </c>
       <c r="J130" s="206">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="K130" s="206">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="L130" s="206">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M130" s="206">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="N130" s="206">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O130" s="206">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="P130" s="206">
-        <f t="shared" ref="P130:T139" si="34">O130</f>
+        <f t="shared" ref="P130:T139" si="35">O130</f>
         <v>0</v>
       </c>
       <c r="Q130" s="206">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="R130" s="206">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="S130" s="206">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="T130" s="206">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="U130" s="206"/>
@@ -51029,55 +51154,55 @@
         <v>1</v>
       </c>
       <c r="H131" s="206">
-        <f t="shared" ref="H131:O139" si="35">G131</f>
+        <f t="shared" ref="H131:O139" si="36">G131</f>
         <v>1</v>
       </c>
       <c r="I131" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="J131" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="K131" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="L131" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="M131" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="N131" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="O131" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="P131" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="J131" s="206">
+      <c r="Q131" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="K131" s="206">
+      <c r="R131" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="L131" s="206">
+      <c r="S131" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="M131" s="206">
+      <c r="T131" s="206">
         <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="N131" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="O131" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="P131" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="Q131" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="R131" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="S131" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="T131" s="206">
-        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="U131" s="206"/>
@@ -51098,55 +51223,55 @@
         <v>0.5</v>
       </c>
       <c r="H132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="I132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="J132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="K132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="L132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="M132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="N132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="O132" s="206">
+        <f t="shared" si="36"/>
+        <v>0.5</v>
+      </c>
+      <c r="P132" s="206">
         <f t="shared" si="35"/>
         <v>0.5</v>
       </c>
-      <c r="I132" s="206">
+      <c r="Q132" s="206">
         <f t="shared" si="35"/>
         <v>0.5</v>
       </c>
-      <c r="J132" s="206">
+      <c r="R132" s="206">
         <f t="shared" si="35"/>
         <v>0.5</v>
       </c>
-      <c r="K132" s="206">
+      <c r="S132" s="206">
         <f t="shared" si="35"/>
         <v>0.5</v>
       </c>
-      <c r="L132" s="206">
+      <c r="T132" s="206">
         <f t="shared" si="35"/>
-        <v>0.5</v>
-      </c>
-      <c r="M132" s="206">
-        <f t="shared" si="35"/>
-        <v>0.5</v>
-      </c>
-      <c r="N132" s="206">
-        <f t="shared" si="35"/>
-        <v>0.5</v>
-      </c>
-      <c r="O132" s="206">
-        <f t="shared" si="35"/>
-        <v>0.5</v>
-      </c>
-      <c r="P132" s="206">
-        <f t="shared" si="34"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q132" s="206">
-        <f t="shared" si="34"/>
-        <v>0.5</v>
-      </c>
-      <c r="R132" s="206">
-        <f t="shared" si="34"/>
-        <v>0.5</v>
-      </c>
-      <c r="S132" s="206">
-        <f t="shared" si="34"/>
-        <v>0.5</v>
-      </c>
-      <c r="T132" s="206">
-        <f t="shared" si="34"/>
         <v>0.5</v>
       </c>
       <c r="U132" s="206"/>
@@ -51167,55 +51292,55 @@
         <v>1</v>
       </c>
       <c r="H133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="I133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="J133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="K133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="L133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="M133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="N133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="O133" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="P133" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="I133" s="206">
+      <c r="Q133" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="J133" s="206">
+      <c r="R133" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="K133" s="206">
+      <c r="S133" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="L133" s="206">
+      <c r="T133" s="206">
         <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="M133" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="N133" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="O133" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="P133" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="Q133" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="R133" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="S133" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="T133" s="206">
-        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="U133" s="206"/>
@@ -51236,55 +51361,55 @@
         <v>1</v>
       </c>
       <c r="H134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="I134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="J134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="K134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="L134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="M134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="N134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="O134" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="P134" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="I134" s="206">
+      <c r="Q134" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="J134" s="206">
+      <c r="R134" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="K134" s="206">
+      <c r="S134" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="L134" s="206">
+      <c r="T134" s="206">
         <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="M134" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="N134" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="O134" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="P134" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="Q134" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="R134" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="S134" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="T134" s="206">
-        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="U134" s="206"/>
@@ -51301,55 +51426,55 @@
         <v>0</v>
       </c>
       <c r="H135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="I135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="J135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="L135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="M135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="N135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="O135" s="211">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="P135" s="211">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="I135" s="211">
+      <c r="Q135" s="211">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="J135" s="211">
+      <c r="R135" s="211">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="K135" s="211">
+      <c r="S135" s="211">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="L135" s="211">
+      <c r="T135" s="211">
         <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="M135" s="211">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="N135" s="211">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="O135" s="211">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="P135" s="211">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="Q135" s="211">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="R135" s="211">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="S135" s="211">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T135" s="211">
-        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -51368,55 +51493,55 @@
         <v>0</v>
       </c>
       <c r="H136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="I136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="J136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="L136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="M136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="N136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="O136" s="206">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="P136" s="206">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="I136" s="206">
+      <c r="Q136" s="206">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="J136" s="206">
+      <c r="R136" s="206">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="K136" s="206">
+      <c r="S136" s="206">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="L136" s="206">
+      <c r="T136" s="206">
         <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="M136" s="206">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="N136" s="206">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="O136" s="206">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="P136" s="206">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="Q136" s="206">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="R136" s="206">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="S136" s="206">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T136" s="206">
-        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="U136" s="206"/>
@@ -51437,55 +51562,55 @@
         <v>1</v>
       </c>
       <c r="H137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="I137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="J137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="K137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="L137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="M137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="N137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="O137" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="P137" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="I137" s="206">
+      <c r="Q137" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="J137" s="206">
+      <c r="R137" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="K137" s="206">
+      <c r="S137" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="L137" s="206">
+      <c r="T137" s="206">
         <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="M137" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="N137" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="O137" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="P137" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="Q137" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="R137" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="S137" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="T137" s="206">
-        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="U137" s="206"/>
@@ -51506,55 +51631,55 @@
         <v>1</v>
       </c>
       <c r="H138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="I138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="J138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="K138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="L138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="M138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="N138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="O138" s="206">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="P138" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="I138" s="206">
+      <c r="Q138" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="J138" s="206">
+      <c r="R138" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="K138" s="206">
+      <c r="S138" s="206">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="L138" s="206">
+      <c r="T138" s="206">
         <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="M138" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="N138" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="O138" s="206">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="P138" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="Q138" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="R138" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="S138" s="206">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="T138" s="206">
-        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="U138" s="206"/>
@@ -51571,55 +51696,55 @@
         <v>0</v>
       </c>
       <c r="H139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="I139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="J139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="L139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="M139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="N139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="O139" s="277">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="P139" s="277">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="I139" s="277">
+      <c r="Q139" s="277">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="J139" s="277">
+      <c r="R139" s="277">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="K139" s="277">
+      <c r="S139" s="277">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="L139" s="277">
+      <c r="T139" s="277">
         <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="M139" s="277">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="N139" s="277">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="O139" s="277">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="P139" s="277">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="Q139" s="277">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="R139" s="277">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="S139" s="277">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T139" s="277">
-        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -51632,63 +51757,63 @@
       <c r="D140" s="204"/>
       <c r="E140" s="204"/>
       <c r="F140" s="204">
-        <f t="shared" ref="F140:T140" si="36">SUM(F130:F139)</f>
+        <f t="shared" ref="F140:T140" si="37">SUM(F130:F139)</f>
         <v>3.5</v>
       </c>
       <c r="G140" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="H140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="I140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="J140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="K140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="L140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="M140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="N140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="O140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="P140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="Q140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="R140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="S140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="T140" s="85">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>5.5</v>
       </c>
       <c r="U140" s="206"/>
@@ -51696,17 +51821,17 @@
     </row>
     <row r="142" spans="1:22" ht="15.75" customHeight="1">
       <c r="F142" s="269"/>
-      <c r="G142" s="371" t="s">
+      <c r="G142" s="372" t="s">
         <v>632</v>
       </c>
-      <c r="H142" s="372"/>
-      <c r="I142" s="372"/>
+      <c r="H142" s="373"/>
+      <c r="I142" s="373"/>
       <c r="K142" s="269"/>
-      <c r="L142" s="371" t="s">
+      <c r="L142" s="372" t="s">
         <v>633</v>
       </c>
-      <c r="M142" s="372"/>
-      <c r="N142" s="372"/>
+      <c r="M142" s="373"/>
+      <c r="N142" s="373"/>
     </row>
     <row r="143" spans="1:22" ht="15.75" customHeight="1">
       <c r="F143" s="272" t="s">
@@ -51976,11 +52101,11 @@
         <v>30</v>
       </c>
       <c r="H151" s="269">
-        <f t="shared" ref="H151:I151" si="37">H150*H143</f>
+        <f t="shared" ref="H151:I151" si="38">H150*H143</f>
         <v>41</v>
       </c>
       <c r="I151" s="269">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>51</v>
       </c>
       <c r="K151" s="185" t="s">
@@ -51991,11 +52116,11 @@
         <v>30</v>
       </c>
       <c r="M151" s="269">
-        <f t="shared" ref="M151" si="38">M150*M143</f>
+        <f t="shared" ref="M151" si="39">M150*M143</f>
         <v>41</v>
       </c>
       <c r="N151" s="269">
-        <f t="shared" ref="N151" si="39">N150*N143</f>
+        <f t="shared" ref="N151" si="40">N150*N143</f>
         <v>51</v>
       </c>
       <c r="P151" s="47" t="s">
@@ -52014,11 +52139,11 @@
         <v>261.60000000000002</v>
       </c>
       <c r="H152" s="270">
-        <f t="shared" ref="H152:I152" si="40">$B$116*H151</f>
+        <f t="shared" ref="H152:I152" si="41">$B$116*H151</f>
         <v>357.52000000000004</v>
       </c>
       <c r="I152" s="270">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>444.72</v>
       </c>
       <c r="K152" s="185" t="s">
@@ -52029,11 +52154,11 @@
         <v>261.60000000000002</v>
       </c>
       <c r="M152" s="270">
-        <f t="shared" ref="M152" si="41">$B$116*M151</f>
+        <f t="shared" ref="M152" si="42">$B$116*M151</f>
         <v>357.52000000000004</v>
       </c>
       <c r="N152" s="270">
-        <f t="shared" ref="N152" si="42">$B$116*N151</f>
+        <f t="shared" ref="N152" si="43">$B$116*N151</f>
         <v>444.72</v>
       </c>
       <c r="P152" s="47" t="s">
@@ -52045,17 +52170,17 @@
     </row>
     <row r="153" spans="6:17" ht="15.75" customHeight="1">
       <c r="F153" s="269"/>
-      <c r="G153" s="371" t="s">
+      <c r="G153" s="372" t="s">
         <v>631</v>
       </c>
-      <c r="H153" s="371"/>
-      <c r="I153" s="371"/>
+      <c r="H153" s="372"/>
+      <c r="I153" s="372"/>
       <c r="K153" s="269"/>
-      <c r="L153" s="371" t="s">
+      <c r="L153" s="372" t="s">
         <v>631</v>
       </c>
-      <c r="M153" s="371"/>
-      <c r="N153" s="371"/>
+      <c r="M153" s="372"/>
+      <c r="N153" s="372"/>
       <c r="P153" s="47" t="s">
         <v>64</v>
       </c>
@@ -52073,11 +52198,11 @@
         <v>130</v>
       </c>
       <c r="H154" s="269">
-        <f t="shared" ref="H154:I154" si="43">H150*52/12</f>
+        <f t="shared" ref="H154:I154" si="44">H150*52/12</f>
         <v>88.833333333333329</v>
       </c>
       <c r="I154" s="269">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>73.666666666666671</v>
       </c>
       <c r="K154" s="185" t="s">
@@ -52088,11 +52213,11 @@
         <v>130</v>
       </c>
       <c r="M154" s="269">
-        <f t="shared" ref="M154:N154" si="44">M150*52/12</f>
+        <f t="shared" ref="M154:N154" si="45">M150*52/12</f>
         <v>88.833333333333329</v>
       </c>
       <c r="N154" s="269">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>73.666666666666671</v>
       </c>
     </row>
@@ -52105,11 +52230,11 @@
         <v>130</v>
       </c>
       <c r="H155" s="269">
-        <f t="shared" ref="H155:I155" si="45">H154*H143</f>
+        <f t="shared" ref="H155:I155" si="46">H154*H143</f>
         <v>177.66666666666666</v>
       </c>
       <c r="I155" s="269">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>221</v>
       </c>
       <c r="K155" s="185" t="s">
@@ -52120,11 +52245,11 @@
         <v>130</v>
       </c>
       <c r="M155" s="269">
-        <f t="shared" ref="M155" si="46">M154*M143</f>
+        <f t="shared" ref="M155" si="47">M154*M143</f>
         <v>177.66666666666666</v>
       </c>
       <c r="N155" s="269">
-        <f t="shared" ref="N155" si="47">N154*N143</f>
+        <f t="shared" ref="N155" si="48">N154*N143</f>
         <v>221</v>
       </c>
     </row>
@@ -52137,11 +52262,11 @@
         <v>1133.6000000000001</v>
       </c>
       <c r="H156" s="270">
-        <f t="shared" ref="H156:I156" si="48">H155*$B$116</f>
+        <f t="shared" ref="H156:I156" si="49">H155*$B$116</f>
         <v>1549.2533333333333</v>
       </c>
       <c r="I156" s="270">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1927.1200000000001</v>
       </c>
       <c r="K156" s="185" t="s">
@@ -52152,11 +52277,11 @@
         <v>1133.6000000000001</v>
       </c>
       <c r="M156" s="270">
-        <f t="shared" ref="M156" si="49">M155*$B$116</f>
+        <f t="shared" ref="M156" si="50">M155*$B$116</f>
         <v>1549.2533333333333</v>
       </c>
       <c r="N156" s="270">
-        <f t="shared" ref="N156" si="50">N155*$B$116</f>
+        <f t="shared" ref="N156" si="51">N155*$B$116</f>
         <v>1927.1200000000001</v>
       </c>
     </row>
@@ -52319,34 +52444,34 @@
       <c r="K1" s="96"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="367" t="s">
+      <c r="A2" s="368" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="367"/>
-      <c r="C2" s="366"/>
-      <c r="D2" s="366"/>
-      <c r="E2" s="366"/>
-      <c r="F2" s="366"/>
-      <c r="G2" s="366"/>
-      <c r="H2" s="366"/>
-      <c r="I2" s="366"/>
-      <c r="J2" s="366"/>
-      <c r="K2" s="366"/>
+      <c r="B2" s="368"/>
+      <c r="C2" s="367"/>
+      <c r="D2" s="367"/>
+      <c r="E2" s="367"/>
+      <c r="F2" s="367"/>
+      <c r="G2" s="367"/>
+      <c r="H2" s="367"/>
+      <c r="I2" s="367"/>
+      <c r="J2" s="367"/>
+      <c r="K2" s="367"/>
     </row>
     <row r="3" spans="1:11" s="96" customFormat="1">
-      <c r="A3" s="368" t="s">
+      <c r="A3" s="369" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="368"/>
-      <c r="C3" s="366"/>
-      <c r="D3" s="366"/>
-      <c r="E3" s="366"/>
-      <c r="F3" s="366"/>
-      <c r="G3" s="366"/>
-      <c r="H3" s="366"/>
-      <c r="I3" s="366"/>
-      <c r="J3" s="366"/>
-      <c r="K3" s="366"/>
+      <c r="B3" s="369"/>
+      <c r="C3" s="367"/>
+      <c r="D3" s="367"/>
+      <c r="E3" s="367"/>
+      <c r="F3" s="367"/>
+      <c r="G3" s="367"/>
+      <c r="H3" s="367"/>
+      <c r="I3" s="367"/>
+      <c r="J3" s="367"/>
+      <c r="K3" s="367"/>
     </row>
     <row r="4" spans="1:11" s="96" customFormat="1">
       <c r="A4" s="92" t="s">
@@ -52364,19 +52489,19 @@
       <c r="K4" s="93"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="369" t="s">
+      <c r="A5" s="370" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="369"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
-      <c r="G5" s="366"/>
-      <c r="H5" s="366"/>
-      <c r="I5" s="366"/>
-      <c r="J5" s="366"/>
-      <c r="K5" s="366"/>
+      <c r="B5" s="370"/>
+      <c r="C5" s="367"/>
+      <c r="D5" s="367"/>
+      <c r="E5" s="367"/>
+      <c r="F5" s="367"/>
+      <c r="G5" s="367"/>
+      <c r="H5" s="367"/>
+      <c r="I5" s="367"/>
+      <c r="J5" s="367"/>
+      <c r="K5" s="367"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="94" t="s">
@@ -52485,12 +52610,12 @@
       <c r="C14" s="98"/>
       <c r="D14" s="98"/>
       <c r="E14" s="98"/>
-      <c r="F14" s="383" t="s">
+      <c r="F14" s="384" t="s">
         <v>262</v>
       </c>
-      <c r="G14" s="383"/>
-      <c r="H14" s="383"/>
-      <c r="I14" s="383"/>
+      <c r="G14" s="384"/>
+      <c r="H14" s="384"/>
+      <c r="I14" s="384"/>
       <c r="J14" s="96"/>
       <c r="K14" s="96"/>
     </row>
@@ -54094,13 +54219,13 @@
     </row>
     <row r="21" spans="1:13" s="160" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="147"/>
-      <c r="B21" s="384" t="s">
+      <c r="B21" s="385" t="s">
         <v>481</v>
       </c>
-      <c r="C21" s="384"/>
-      <c r="D21" s="384"/>
-      <c r="E21" s="384"/>
-      <c r="F21" s="384"/>
+      <c r="C21" s="385"/>
+      <c r="D21" s="385"/>
+      <c r="E21" s="385"/>
+      <c r="F21" s="385"/>
       <c r="G21" s="55"/>
       <c r="H21" s="55"/>
       <c r="I21" s="55"/>
@@ -54300,13 +54425,13 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
       <c r="A33" s="147"/>
-      <c r="B33" s="384" t="s">
+      <c r="B33" s="385" t="s">
         <v>481</v>
       </c>
-      <c r="C33" s="384"/>
-      <c r="D33" s="384"/>
-      <c r="E33" s="384"/>
-      <c r="F33" s="384"/>
+      <c r="C33" s="385"/>
+      <c r="D33" s="385"/>
+      <c r="E33" s="385"/>
+      <c r="F33" s="385"/>
       <c r="H33" s="55"/>
       <c r="I33" s="55"/>
       <c r="J33" s="55"/>
@@ -56611,14 +56736,14 @@
       <c r="G6" s="149"/>
       <c r="H6" s="149"/>
       <c r="I6" s="149"/>
-      <c r="J6" s="385" t="s">
+      <c r="J6" s="386" t="s">
         <v>465</v>
       </c>
-      <c r="K6" s="385"/>
-      <c r="L6" s="385"/>
-      <c r="M6" s="385"/>
-      <c r="N6" s="385"/>
-      <c r="O6" s="385"/>
+      <c r="K6" s="386"/>
+      <c r="L6" s="386"/>
+      <c r="M6" s="386"/>
+      <c r="N6" s="386"/>
+      <c r="O6" s="386"/>
       <c r="P6" s="153"/>
       <c r="Q6" s="153"/>
     </row>
@@ -67608,12 +67733,12 @@
       <c r="C19" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="386" t="s">
+      <c r="G19" s="387" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="386"/>
-      <c r="I19" s="386"/>
-      <c r="J19" s="386"/>
+      <c r="H19" s="387"/>
+      <c r="I19" s="387"/>
+      <c r="J19" s="387"/>
       <c r="L19" s="30" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
Added risks - pests, electrical blackout, laour challenges, planning permission delays Added opportunities for lighting efficiency improvements Added scenario parameters for pest outbreaks and electrical back-up Stub for HVAC energy estimation
</commit_message>
<xml_diff>
--- a/Current_Financial_Model.xlsx
+++ b/Current_Financial_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Francis/PycharmProjects/VerticalFarming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4340A06-5EBB-D846-9BC9-C0A1A36C3932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15217002-06B2-BA41-9954-12948D157AE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="21360" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24400" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="14" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="ceo_msalary">Overview!$B$120</definedName>
     <definedName name="climate_control">Overview!$B$33</definedName>
     <definedName name="co2_enrichment">Overview!$B$43</definedName>
-    <definedName name="construction_cost">Overview!$B$60</definedName>
+    <definedName name="construction_cost">Overview!$B$62</definedName>
     <definedName name="crop_total_percent">Overview!$L$16</definedName>
     <definedName name="crop_typ1">Overview!$H$15</definedName>
     <definedName name="crop_typ2">Overview!$I$15</definedName>
@@ -161,7 +161,7 @@
     <definedName name="education_avg_revenue_y2">Overview!$G$77</definedName>
     <definedName name="education_multiplier">Overview!$C$77</definedName>
     <definedName name="electricity_price">Overview!$B$46</definedName>
-    <definedName name="equipment_cost">Overview!$B$61</definedName>
+    <definedName name="equipment_cost">Overview!$B$63</definedName>
     <definedName name="facility_size_full">Overview!$C$15</definedName>
     <definedName name="facility_size_pilot">Overview!$B$15</definedName>
     <definedName name="farm_type">Overview!$B$29</definedName>
@@ -199,14 +199,15 @@
     <definedName name="insultation_level">Overview!$B$41</definedName>
     <definedName name="insurance_full">Overview!$G$98</definedName>
     <definedName name="insurance_pilot">Overview!$F$98</definedName>
+    <definedName name="ipm">Overview!$B$50</definedName>
     <definedName name="labour_improvement">Overview!$B$47</definedName>
     <definedName name="light_qty">Overview!$C$37</definedName>
     <definedName name="light_system">Overview!$B$37</definedName>
     <definedName name="lighting_control">Overview!$B$34</definedName>
-    <definedName name="loan_amount">Overview!$B$53</definedName>
-    <definedName name="loan_interest">Overview!$B$55</definedName>
-    <definedName name="loan_tenure">Overview!$B$56</definedName>
-    <definedName name="loan_type">Overview!$B$57</definedName>
+    <definedName name="loan_amount">Overview!$B$55</definedName>
+    <definedName name="loan_interest">Overview!$B$57</definedName>
+    <definedName name="loan_tenure">Overview!$B$58</definedName>
+    <definedName name="loan_type">Overview!$B$59</definedName>
     <definedName name="m1_wa_sales">Overview!$F$72</definedName>
     <definedName name="m1_wa_yield_crop1">Overview!$F$68</definedName>
     <definedName name="m1_wa_yield_crop2">Overview!$F$69</definedName>
@@ -261,6 +262,7 @@
     <definedName name="percent_production_area_full">Overview!$C$16</definedName>
     <definedName name="percent_production_area_pilot">Overview!$B$16</definedName>
     <definedName name="percentage_renewable_energy">Overview!$B$48</definedName>
+    <definedName name="pest_detection">Overview!$B$51</definedName>
     <definedName name="plant_sites">Overview!$B$38</definedName>
     <definedName name="production_area_full">Overview!$C$16</definedName>
     <definedName name="production_area_pilot">Overview!$B$16</definedName>
@@ -273,7 +275,7 @@
     <definedName name="productivity_volume">Overview!$I$51</definedName>
     <definedName name="productivity_water">Overview!$I$49</definedName>
     <definedName name="produticity_net_CO2">Overview!$I$54</definedName>
-    <definedName name="reserve_fund">Overview!$B$63</definedName>
+    <definedName name="reserve_fund">Overview!$B$65</definedName>
     <definedName name="roof_type">Overview!$B$42</definedName>
     <definedName name="salesperson_count_y1">Overview!$F$134</definedName>
     <definedName name="salesperson_count_y2">Overview!$G$134</definedName>
@@ -297,12 +299,12 @@
     <definedName name="target_productivity_space">Overview!$J$46</definedName>
     <definedName name="target_productivity_volume">Overview!$J$51</definedName>
     <definedName name="target_productivity_water">Overview!$J$49</definedName>
-    <definedName name="tax_rate">Overview!$B$54</definedName>
+    <definedName name="tax_rate">Overview!$B$56</definedName>
     <definedName name="total_brevenue_full">Overview!$L$28</definedName>
     <definedName name="total_brevenue_pilot">Overview!$L$27</definedName>
     <definedName name="total_byield_full">Overview!$L$26</definedName>
     <definedName name="total_byield_pilot">Overview!$L$25</definedName>
-    <definedName name="total_capex">Overview!$B$62</definedName>
+    <definedName name="total_capex">Overview!$B$64</definedName>
     <definedName name="total_headcount_y1">Overview!$F$140</definedName>
     <definedName name="total_headcount_y2">Overview!$G$140</definedName>
     <definedName name="total_plants_full">Overview!$L$30</definedName>
@@ -1925,7 +1927,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="886">
   <si>
     <t>Packaging types &amp; ROUGH Cost per package</t>
   </si>
@@ -4568,6 +4570,21 @@
   </si>
   <si>
     <t>target_productivity_CO2_miti</t>
+  </si>
+  <si>
+    <t>Integrated Pest Management</t>
+  </si>
+  <si>
+    <t>Pest Detection Technology</t>
+  </si>
+  <si>
+    <t>ipm</t>
+  </si>
+  <si>
+    <t>pest_detection</t>
+  </si>
+  <si>
+    <t>electrical_backup</t>
   </si>
 </sst>
 </file>
@@ -5390,7 +5407,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="388">
+  <cellXfs count="390">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -5902,6 +5919,8 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -14217,10 +14236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1FB0-CD2F-E14E-8300-C92D3DA9F93F}">
-  <dimension ref="A1:B128"/>
+  <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="96" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -15375,6 +15394,32 @@
       <c r="B128">
         <f>target_productivity_CO2_net</f>
         <v>-100</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="47" t="s">
+        <v>883</v>
+      </c>
+      <c r="B129" t="str">
+        <f>ipm</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="47" t="s">
+        <v>884</v>
+      </c>
+      <c r="B130" t="str">
+        <f>pest_detection</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="47" t="s">
+        <v>885</v>
+      </c>
+      <c r="B131" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -16349,63 +16394,63 @@
         <v>-2141.0728711398056</v>
       </c>
       <c r="D18" s="78">
-        <f>D12-(D12*Overview!$B$54)-D14-D16</f>
+        <f>D12-(D12*Overview!$B$56)-D14-D16</f>
         <v>-54183.002379510188</v>
       </c>
       <c r="E18" s="78">
-        <f>E12-(E12*Overview!$B$54)-E14-E16</f>
+        <f>E12-(E12*Overview!$B$56)-E14-E16</f>
         <v>-11064.487365538342</v>
       </c>
       <c r="F18" s="78">
-        <f>F12-(F12*Overview!$B$54)-F14-F16</f>
+        <f>F12-(F12*Overview!$B$56)-F14-F16</f>
         <v>-7680.940875406639</v>
       </c>
       <c r="G18" s="78">
-        <f>G12-(G12*Overview!$B$54)-G14-G16</f>
+        <f>G12-(G12*Overview!$B$56)-G14-G16</f>
         <v>-5249.0168356245849</v>
       </c>
       <c r="H18" s="78">
-        <f>H12-(H12*Overview!$B$54)-H14-H16</f>
+        <f>H12-(H12*Overview!$B$56)-H14-H16</f>
         <v>-3007.4172859122918</v>
       </c>
       <c r="I18" s="78">
-        <f>I12-(I12*Overview!$B$54)-I14-I16</f>
+        <f>I12-(I12*Overview!$B$56)-I14-I16</f>
         <v>27533.985699562461</v>
       </c>
       <c r="J18" s="78">
-        <f>J12-(J12*Overview!$B$54)-J14-J16</f>
+        <f>J12-(J12*Overview!$B$56)-J14-J16</f>
         <v>29437.230600261497</v>
       </c>
       <c r="K18" s="78">
-        <f>K12-(K12*Overview!$B$54)-K14-K16</f>
+        <f>K12-(K12*Overview!$B$56)-K14-K16</f>
         <v>30748.354865187594</v>
       </c>
       <c r="L18" s="78">
-        <f>L12-(L12*Overview!$B$54)-L14-L16</f>
+        <f>L12-(L12*Overview!$B$56)-L14-L16</f>
         <v>31974.890467860259</v>
       </c>
       <c r="M18" s="78">
-        <f>M12-(M12*Overview!$B$54)-M14-M16</f>
+        <f>M12-(M12*Overview!$B$56)-M14-M16</f>
         <v>33137.984573843059</v>
       </c>
       <c r="N18" s="78">
-        <f>N12-(N12*Overview!$B$54)-N14-N16</f>
+        <f>N12-(N12*Overview!$B$56)-N14-N16</f>
         <v>34216.49001757252</v>
       </c>
       <c r="O18" s="78">
-        <f>O12-(O12*Overview!$B$54)-O14-O16</f>
+        <f>O12-(O12*Overview!$B$56)-O14-O16</f>
         <v>35231.553964611972</v>
       </c>
       <c r="P18" s="78">
-        <f>P12-(P12*Overview!$B$54)-P14-P16</f>
+        <f>P12-(P12*Overview!$B$56)-P14-P16</f>
         <v>36204.323580524811</v>
       </c>
       <c r="Q18" s="78">
-        <f>Q12-(Q12*Overview!$B$54)-Q14-Q16</f>
+        <f>Q12-(Q12*Overview!$B$56)-Q14-Q16</f>
         <v>37113.651699747701</v>
       </c>
       <c r="R18" s="78">
-        <f>R12-(R12*Overview!$B$54)-R14-R16</f>
+        <f>R12-(R12*Overview!$B$56)-R14-R16</f>
         <v>37959.538322280612</v>
       </c>
       <c r="S18" s="1"/>
@@ -45257,8 +45302,8 @@
   </sheetPr>
   <dimension ref="A1:V156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -45277,26 +45322,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="13">
-      <c r="A1" s="366" t="s">
+      <c r="A1" s="368" t="s">
         <v>518</v>
       </c>
-      <c r="B1" s="367"/>
-      <c r="C1" s="367"/>
-      <c r="D1" s="367"/>
-      <c r="E1" s="367"/>
-      <c r="F1" s="367"/>
-      <c r="G1" s="367"/>
-      <c r="H1" s="367"/>
+      <c r="B1" s="369"/>
+      <c r="C1" s="369"/>
+      <c r="D1" s="369"/>
+      <c r="E1" s="369"/>
+      <c r="F1" s="369"/>
+      <c r="G1" s="369"/>
+      <c r="H1" s="369"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A2" s="367"/>
-      <c r="B2" s="367"/>
-      <c r="C2" s="367"/>
-      <c r="D2" s="367"/>
-      <c r="E2" s="367"/>
-      <c r="F2" s="367"/>
-      <c r="G2" s="367"/>
-      <c r="H2" s="367"/>
+      <c r="A2" s="369"/>
+      <c r="B2" s="369"/>
+      <c r="C2" s="369"/>
+      <c r="D2" s="369"/>
+      <c r="E2" s="369"/>
+      <c r="F2" s="369"/>
+      <c r="G2" s="369"/>
+      <c r="H2" s="369"/>
     </row>
     <row r="3" spans="1:22" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="59" t="s">
@@ -45304,28 +45349,28 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="13">
-      <c r="A4" s="368" t="s">
+      <c r="A4" s="370" t="s">
         <v>517</v>
       </c>
-      <c r="B4" s="367"/>
-      <c r="C4" s="367"/>
-      <c r="D4" s="367"/>
-      <c r="E4" s="367"/>
-      <c r="F4" s="367"/>
-      <c r="G4" s="367"/>
-      <c r="H4" s="367"/>
+      <c r="B4" s="369"/>
+      <c r="C4" s="369"/>
+      <c r="D4" s="369"/>
+      <c r="E4" s="369"/>
+      <c r="F4" s="369"/>
+      <c r="G4" s="369"/>
+      <c r="H4" s="369"/>
     </row>
     <row r="5" spans="1:22" ht="13">
-      <c r="A5" s="369" t="s">
+      <c r="A5" s="371" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="367"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
-      <c r="G5" s="367"/>
-      <c r="H5" s="367"/>
+      <c r="B5" s="369"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
+      <c r="G5" s="369"/>
+      <c r="H5" s="369"/>
     </row>
     <row r="6" spans="1:22" s="26" customFormat="1" ht="13">
       <c r="A6" s="92" t="s">
@@ -45340,16 +45385,16 @@
       <c r="H6" s="93"/>
     </row>
     <row r="7" spans="1:22" ht="13">
-      <c r="A7" s="370" t="s">
+      <c r="A7" s="372" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="367"/>
-      <c r="C7" s="367"/>
-      <c r="D7" s="367"/>
-      <c r="E7" s="367"/>
-      <c r="F7" s="367"/>
-      <c r="G7" s="367"/>
-      <c r="H7" s="367"/>
+      <c r="B7" s="369"/>
+      <c r="C7" s="369"/>
+      <c r="D7" s="369"/>
+      <c r="E7" s="369"/>
+      <c r="F7" s="369"/>
+      <c r="G7" s="369"/>
+      <c r="H7" s="369"/>
     </row>
     <row r="8" spans="1:22" s="26" customFormat="1" ht="13">
       <c r="A8" s="256" t="s">
@@ -45413,8 +45458,8 @@
       <c r="Q13" s="218"/>
       <c r="R13" s="219"/>
       <c r="S13" s="219"/>
-      <c r="T13" s="365"/>
-      <c r="U13" s="365"/>
+      <c r="T13" s="367"/>
+      <c r="U13" s="367"/>
     </row>
     <row r="14" spans="1:22" ht="16">
       <c r="A14" s="2" t="s">
@@ -45599,7 +45644,7 @@
       </c>
       <c r="D18" s="269"/>
       <c r="E18" s="269"/>
-      <c r="F18" s="372" t="s">
+      <c r="F18" s="374" t="s">
         <v>618</v>
       </c>
       <c r="G18" s="323" t="s">
@@ -45650,7 +45695,7 @@
       </c>
       <c r="D19" s="269"/>
       <c r="E19" s="269"/>
-      <c r="F19" s="372"/>
+      <c r="F19" s="374"/>
       <c r="G19" s="292" t="s">
         <v>585</v>
       </c>
@@ -45797,7 +45842,7 @@
       </c>
       <c r="D23" s="269"/>
       <c r="E23" s="269"/>
-      <c r="F23" s="381" t="s">
+      <c r="F23" s="383" t="s">
         <v>316</v>
       </c>
       <c r="G23" s="326" t="s">
@@ -45829,7 +45874,7 @@
       </c>
       <c r="D24" s="269"/>
       <c r="E24" s="269"/>
-      <c r="F24" s="381"/>
+      <c r="F24" s="383"/>
       <c r="G24" s="326" t="s">
         <v>596</v>
       </c>
@@ -45861,7 +45906,7 @@
       </c>
       <c r="D25" s="269"/>
       <c r="E25" s="269"/>
-      <c r="F25" s="380" t="s">
+      <c r="F25" s="382" t="s">
         <v>542</v>
       </c>
       <c r="G25" s="323" t="s">
@@ -45902,7 +45947,7 @@
       </c>
       <c r="D26" s="269"/>
       <c r="E26" s="269"/>
-      <c r="F26" s="380"/>
+      <c r="F26" s="382"/>
       <c r="G26" s="323" t="s">
         <v>315</v>
       </c>
@@ -45931,7 +45976,7 @@
       <c r="A27" s="4"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
-      <c r="F27" s="378" t="s">
+      <c r="F27" s="380" t="s">
         <v>588</v>
       </c>
       <c r="G27" s="185" t="s">
@@ -45964,7 +46009,7 @@
       </c>
       <c r="B28" s="54"/>
       <c r="C28" s="47"/>
-      <c r="F28" s="379"/>
+      <c r="F28" s="381"/>
       <c r="G28" s="185" t="s">
         <v>315</v>
       </c>
@@ -45997,7 +46042,7 @@
         <v>79</v>
       </c>
       <c r="C29" s="47"/>
-      <c r="F29" s="382" t="s">
+      <c r="F29" s="384" t="s">
         <v>587</v>
       </c>
       <c r="G29" s="185" t="s">
@@ -46032,7 +46077,7 @@
         <v>865</v>
       </c>
       <c r="C30" s="170"/>
-      <c r="F30" s="379"/>
+      <c r="F30" s="381"/>
       <c r="G30" s="185" t="s">
         <v>483</v>
       </c>
@@ -46065,7 +46110,7 @@
         <v>165</v>
       </c>
       <c r="C31" s="170"/>
-      <c r="F31" s="374" t="s">
+      <c r="F31" s="376" t="s">
         <v>531</v>
       </c>
       <c r="G31" s="212" t="s">
@@ -46097,7 +46142,7 @@
         <v>164</v>
       </c>
       <c r="C32" s="170"/>
-      <c r="F32" s="375"/>
+      <c r="F32" s="377"/>
       <c r="G32" s="212" t="s">
         <v>315</v>
       </c>
@@ -46156,7 +46201,7 @@
       <c r="B34" s="356" t="s">
         <v>165</v>
       </c>
-      <c r="F34" s="371" t="s">
+      <c r="F34" s="373" t="s">
         <v>615</v>
       </c>
       <c r="G34" s="185" t="s">
@@ -46190,7 +46235,7 @@
       <c r="C35" s="254" t="s">
         <v>489</v>
       </c>
-      <c r="F35" s="371"/>
+      <c r="F35" s="373"/>
       <c r="G35" s="185" t="s">
         <v>533</v>
       </c>
@@ -46222,7 +46267,7 @@
       <c r="C36" s="264">
         <v>8</v>
       </c>
-      <c r="F36" s="371"/>
+      <c r="F36" s="373"/>
       <c r="G36" s="185" t="s">
         <v>534</v>
       </c>
@@ -46255,7 +46300,7 @@
         <f>C36*16</f>
         <v>128</v>
       </c>
-      <c r="F37" s="371"/>
+      <c r="F37" s="373"/>
       <c r="G37" s="185" t="s">
         <v>535</v>
       </c>
@@ -46286,7 +46331,7 @@
         <f>C36*VLOOKUP(B36, Database!A97:I107, 5, FALSE)</f>
         <v>2880</v>
       </c>
-      <c r="F38" s="371"/>
+      <c r="F38" s="373"/>
       <c r="G38" s="185" t="s">
         <v>536</v>
       </c>
@@ -46316,7 +46361,7 @@
         <v>507</v>
       </c>
       <c r="C39" s="170"/>
-      <c r="F39" s="376" t="s">
+      <c r="F39" s="378" t="s">
         <v>589</v>
       </c>
       <c r="G39" s="212" t="s">
@@ -46348,7 +46393,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="170"/>
-      <c r="F40" s="377"/>
+      <c r="F40" s="379"/>
       <c r="G40" s="212" t="s">
         <v>315</v>
       </c>
@@ -46382,7 +46427,7 @@
       </c>
       <c r="C41" s="170"/>
       <c r="D41" s="55"/>
-      <c r="F41" s="372" t="s">
+      <c r="F41" s="374" t="s">
         <v>613</v>
       </c>
       <c r="G41" s="292" t="s">
@@ -46413,7 +46458,7 @@
         <v>166</v>
       </c>
       <c r="C42" s="170"/>
-      <c r="F42" s="372"/>
+      <c r="F42" s="374"/>
       <c r="G42" s="212" t="s">
         <v>614</v>
       </c>
@@ -46451,11 +46496,11 @@
         <v>722</v>
       </c>
       <c r="C44" s="170"/>
-      <c r="G44" s="383" t="s">
+      <c r="G44" s="385" t="s">
         <v>602</v>
       </c>
-      <c r="H44" s="383"/>
-      <c r="I44" s="383"/>
+      <c r="H44" s="385"/>
+      <c r="I44" s="385"/>
     </row>
     <row r="45" spans="1:12" s="160" customFormat="1" ht="16">
       <c r="A45" s="171" t="s">
@@ -46618,6 +46663,12 @@
       </c>
     </row>
     <row r="50" spans="1:12" s="26" customFormat="1" ht="13">
+      <c r="A50" s="366" t="s">
+        <v>881</v>
+      </c>
+      <c r="B50" s="365" t="s">
+        <v>540</v>
+      </c>
       <c r="C50" s="54"/>
       <c r="F50" s="185" t="s">
         <v>607</v>
@@ -46644,8 +46695,12 @@
       </c>
     </row>
     <row r="51" spans="1:12" s="96" customFormat="1" ht="13">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="366" t="s">
+        <v>882</v>
+      </c>
+      <c r="B51" s="365" t="s">
+        <v>540</v>
+      </c>
       <c r="C51" s="54"/>
       <c r="F51" s="185" t="s">
         <v>608</v>
@@ -46672,11 +46727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="26" customFormat="1" ht="16">
-      <c r="A52" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B52" s="60"/>
+    <row r="52" spans="1:12" s="26" customFormat="1" ht="13">
       <c r="C52" s="54"/>
       <c r="D52" s="55"/>
       <c r="E52" s="55"/>
@@ -46705,13 +46756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="26" customFormat="1" ht="16">
-      <c r="A53" s="245" t="s">
-        <v>211</v>
-      </c>
-      <c r="B53" s="246">
-        <v>108000</v>
-      </c>
+    <row r="53" spans="1:12" s="26" customFormat="1" ht="13">
       <c r="D53" s="6"/>
       <c r="E53" s="48"/>
       <c r="F53" s="185" t="s">
@@ -46740,12 +46785,10 @@
       </c>
     </row>
     <row r="54" spans="1:12" s="26" customFormat="1" ht="16">
-      <c r="A54" s="247" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="248">
-        <v>0</v>
-      </c>
+      <c r="A54" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B54" s="60"/>
       <c r="C54" s="48"/>
       <c r="D54" s="6"/>
       <c r="E54" s="48"/>
@@ -46775,11 +46818,11 @@
       </c>
     </row>
     <row r="55" spans="1:12" s="26" customFormat="1" ht="16">
-      <c r="A55" s="247" t="s">
-        <v>210</v>
-      </c>
-      <c r="B55" s="248">
-        <v>0.1</v>
+      <c r="A55" s="245" t="s">
+        <v>211</v>
+      </c>
+      <c r="B55" s="246">
+        <v>108000</v>
       </c>
       <c r="C55" s="48"/>
       <c r="D55" s="6"/>
@@ -46811,10 +46854,10 @@
     </row>
     <row r="56" spans="1:12" ht="16">
       <c r="A56" s="247" t="s">
-        <v>212</v>
-      </c>
-      <c r="B56" s="249">
-        <v>5</v>
+        <v>72</v>
+      </c>
+      <c r="B56" s="248">
+        <v>0</v>
       </c>
       <c r="C56" s="48"/>
       <c r="D56" s="26"/>
@@ -46827,17 +46870,21 @@
     </row>
     <row r="57" spans="1:12" s="28" customFormat="1" ht="16">
       <c r="A57" s="247" t="s">
-        <v>217</v>
-      </c>
-      <c r="B57" s="249" t="s">
-        <v>218</v>
+        <v>210</v>
+      </c>
+      <c r="B57" s="248">
+        <v>0.1</v>
       </c>
       <c r="C57" s="54"/>
       <c r="J57" s="26"/>
     </row>
-    <row r="58" spans="1:12" s="102" customFormat="1" ht="13">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
+    <row r="58" spans="1:12" s="102" customFormat="1" ht="16">
+      <c r="A58" s="247" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="249">
+        <v>5</v>
+      </c>
       <c r="C58" s="54"/>
       <c r="I58" s="102">
         <f>SUM(V68:V71)</f>
@@ -46846,30 +46893,24 @@
       <c r="J58" s="26"/>
     </row>
     <row r="59" spans="1:12" s="28" customFormat="1" ht="16">
-      <c r="A59" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B59" s="6"/>
+      <c r="A59" s="247" t="s">
+        <v>217</v>
+      </c>
+      <c r="B59" s="249" t="s">
+        <v>218</v>
+      </c>
       <c r="C59" s="54"/>
       <c r="J59"/>
     </row>
     <row r="60" spans="1:12" s="28" customFormat="1" ht="13">
-      <c r="A60" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="48">
-        <f>'CapEx Breakdown'!C21+'CapEx Breakdown'!D21</f>
-        <v>49362.593242414143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="128" customFormat="1" ht="13">
-      <c r="A61" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B61" s="48">
-        <f>'CapEx Breakdown'!C34+'CapEx Breakdown'!D34</f>
-        <v>173745.03729696566</v>
-      </c>
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+    </row>
+    <row r="61" spans="1:12" s="128" customFormat="1" ht="16">
+      <c r="A61" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="6"/>
       <c r="C61" s="28"/>
       <c r="J61" s="102">
         <f>1-0.4-0.002</f>
@@ -46878,26 +46919,42 @@
     </row>
     <row r="62" spans="1:12" s="128" customFormat="1" ht="13">
       <c r="A62" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="48">
+        <f>'CapEx Breakdown'!C21+'CapEx Breakdown'!D21</f>
+        <v>49362.593242414143</v>
+      </c>
+      <c r="J62" s="28"/>
+    </row>
+    <row r="63" spans="1:12" s="128" customFormat="1" ht="13">
+      <c r="A63" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="48">
+        <f>'CapEx Breakdown'!C34+'CapEx Breakdown'!D34</f>
+        <v>173745.03729696566</v>
+      </c>
+      <c r="J63" s="28"/>
+    </row>
+    <row r="64" spans="1:12" s="28" customFormat="1" ht="13">
+      <c r="A64" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="91">
+      <c r="B64" s="91">
         <f>'CapEx Breakdown'!E37</f>
         <v>223107.63053937981</v>
       </c>
-      <c r="J62" s="28"/>
-    </row>
-    <row r="63" spans="1:12" s="128" customFormat="1" ht="13">
-      <c r="A63" s="159" t="s">
+    </row>
+    <row r="65" spans="1:22" s="128" customFormat="1" ht="13">
+      <c r="A65" s="159" t="s">
         <v>634</v>
       </c>
-      <c r="B63" s="106">
-        <f>B53-B62</f>
+      <c r="B65" s="106">
+        <f>B55-B64</f>
         <v>-115107.63053937981</v>
       </c>
-      <c r="J63" s="28"/>
-    </row>
-    <row r="64" spans="1:12" s="28" customFormat="1" ht="13"/>
-    <row r="65" spans="1:22" s="128" customFormat="1" ht="13"/>
+    </row>
     <row r="66" spans="1:22" s="128" customFormat="1" ht="13"/>
     <row r="67" spans="1:22" s="28" customFormat="1" ht="16">
       <c r="A67" s="2" t="s">
@@ -49425,19 +49482,19 @@
         <v>2374.1773271527068</v>
       </c>
       <c r="H104" s="78">
-        <f>IF($B$56/H73&gt;=1,  (Overview!$B$55*Overview!$B$53)/(1-(1+Overview!$B$55)^(-Overview!$B$56)), 0)</f>
+        <f>IF($B$58/H73&gt;=1,  (Overview!$B$57*Overview!$B$55)/(1-(1+Overview!$B$57)^(-Overview!$B$58)), 0)</f>
         <v>28490.127925832483</v>
       </c>
       <c r="I104" s="78">
-        <f>IF($B$56/I73&gt;=1, H104, 0)</f>
+        <f t="shared" ref="I104:V104" si="19">IF($B$58/I73&gt;=1, H104, 0)</f>
         <v>28490.127925832483</v>
       </c>
       <c r="J104" s="78">
-        <f>IF($B$56/J73&gt;=1, I104, 0)</f>
+        <f t="shared" si="19"/>
         <v>28490.127925832483</v>
       </c>
       <c r="K104" s="78">
-        <f t="shared" ref="K104:V104" si="19">IF($B$56/K73&gt;=1, J104, 0)</f>
+        <f t="shared" si="19"/>
         <v>28490.127925832483</v>
       </c>
       <c r="L104" s="78">
@@ -49494,7 +49551,7 @@
       <c r="D105" s="206"/>
       <c r="E105" s="206"/>
       <c r="F105" s="81">
-        <f>-(Overview!$B$53)</f>
+        <f>-(Overview!$B$55)</f>
         <v>-108000</v>
       </c>
       <c r="G105" s="196">
@@ -49502,15 +49559,15 @@
         <v>-90309.872074167521</v>
       </c>
       <c r="H105" s="81">
-        <f>F105+H104+(F105*$B$55)</f>
+        <f>F105+H104+(F105*$B$57)</f>
         <v>-90309.872074167521</v>
       </c>
       <c r="I105" s="81">
-        <f t="shared" ref="I105:V105" si="20">H105+I104+(H105*$B$55)</f>
+        <f t="shared" ref="I105:V105" si="20">H105+I104+(H105*$B$57)</f>
         <v>-70850.731355751792</v>
       </c>
       <c r="J105" s="81">
-        <f>I105+J104+(I105*$B$55)</f>
+        <f t="shared" si="20"/>
         <v>-49445.67656549449</v>
       </c>
       <c r="K105" s="81">
@@ -49573,7 +49630,7 @@
       <c r="F106" s="90"/>
       <c r="G106" s="206"/>
       <c r="H106" s="90">
-        <f t="shared" ref="H106:V106" si="21">$B$54*H102</f>
+        <f t="shared" ref="H106:V106" si="21">$B$56*H102</f>
         <v>0</v>
       </c>
       <c r="I106" s="90">
@@ -51821,17 +51878,17 @@
     </row>
     <row r="142" spans="1:22" ht="15.75" customHeight="1">
       <c r="F142" s="269"/>
-      <c r="G142" s="372" t="s">
+      <c r="G142" s="374" t="s">
         <v>632</v>
       </c>
-      <c r="H142" s="373"/>
-      <c r="I142" s="373"/>
+      <c r="H142" s="375"/>
+      <c r="I142" s="375"/>
       <c r="K142" s="269"/>
-      <c r="L142" s="372" t="s">
+      <c r="L142" s="374" t="s">
         <v>633</v>
       </c>
-      <c r="M142" s="373"/>
-      <c r="N142" s="373"/>
+      <c r="M142" s="375"/>
+      <c r="N142" s="375"/>
     </row>
     <row r="143" spans="1:22" ht="15.75" customHeight="1">
       <c r="F143" s="272" t="s">
@@ -52170,17 +52227,17 @@
     </row>
     <row r="153" spans="6:17" ht="15.75" customHeight="1">
       <c r="F153" s="269"/>
-      <c r="G153" s="372" t="s">
+      <c r="G153" s="374" t="s">
         <v>631</v>
       </c>
-      <c r="H153" s="372"/>
-      <c r="I153" s="372"/>
+      <c r="H153" s="374"/>
+      <c r="I153" s="374"/>
       <c r="K153" s="269"/>
-      <c r="L153" s="372" t="s">
+      <c r="L153" s="374" t="s">
         <v>631</v>
       </c>
-      <c r="M153" s="372"/>
-      <c r="N153" s="372"/>
+      <c r="M153" s="374"/>
+      <c r="N153" s="374"/>
       <c r="P153" s="47" t="s">
         <v>64</v>
       </c>
@@ -52332,7 +52389,7 @@
       <formula>$B$40*2.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41 B31:B32 B49" xr:uid="{7D71A6BF-D46C-2B45-AA0C-5B85E55589B2}">
       <formula1>"High, Medium, Low"</formula1>
     </dataValidation>
@@ -52349,11 +52406,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42" xr:uid="{6FA659DB-36A0-DB41-BC4B-A98B31225F76}">
       <formula1>"Pitched roof, Flat roof"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57" xr:uid="{A459DD22-BA10-A141-9360-472E62E9697B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59" xr:uid="{A459DD22-BA10-A141-9360-472E62E9697B}">
       <formula1>"Standard"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30" xr:uid="{EF0D7628-D52D-C04B-9260-03EC3F18C0B2}">
       <formula1>"Retail, Wholesale, Hybrid"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50:B51" xr:uid="{687EBD68-1C3F-8C4B-AE82-97178D4132B8}">
+      <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -52444,34 +52504,34 @@
       <c r="K1" s="96"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="368" t="s">
+      <c r="A2" s="370" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="368"/>
-      <c r="C2" s="367"/>
-      <c r="D2" s="367"/>
-      <c r="E2" s="367"/>
-      <c r="F2" s="367"/>
-      <c r="G2" s="367"/>
-      <c r="H2" s="367"/>
-      <c r="I2" s="367"/>
-      <c r="J2" s="367"/>
-      <c r="K2" s="367"/>
+      <c r="B2" s="370"/>
+      <c r="C2" s="369"/>
+      <c r="D2" s="369"/>
+      <c r="E2" s="369"/>
+      <c r="F2" s="369"/>
+      <c r="G2" s="369"/>
+      <c r="H2" s="369"/>
+      <c r="I2" s="369"/>
+      <c r="J2" s="369"/>
+      <c r="K2" s="369"/>
     </row>
     <row r="3" spans="1:11" s="96" customFormat="1">
-      <c r="A3" s="369" t="s">
+      <c r="A3" s="371" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="369"/>
-      <c r="C3" s="367"/>
-      <c r="D3" s="367"/>
-      <c r="E3" s="367"/>
-      <c r="F3" s="367"/>
-      <c r="G3" s="367"/>
-      <c r="H3" s="367"/>
-      <c r="I3" s="367"/>
-      <c r="J3" s="367"/>
-      <c r="K3" s="367"/>
+      <c r="B3" s="371"/>
+      <c r="C3" s="369"/>
+      <c r="D3" s="369"/>
+      <c r="E3" s="369"/>
+      <c r="F3" s="369"/>
+      <c r="G3" s="369"/>
+      <c r="H3" s="369"/>
+      <c r="I3" s="369"/>
+      <c r="J3" s="369"/>
+      <c r="K3" s="369"/>
     </row>
     <row r="4" spans="1:11" s="96" customFormat="1">
       <c r="A4" s="92" t="s">
@@ -52489,19 +52549,19 @@
       <c r="K4" s="93"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="370" t="s">
+      <c r="A5" s="372" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="370"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
-      <c r="G5" s="367"/>
-      <c r="H5" s="367"/>
-      <c r="I5" s="367"/>
-      <c r="J5" s="367"/>
-      <c r="K5" s="367"/>
+      <c r="B5" s="372"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
+      <c r="G5" s="369"/>
+      <c r="H5" s="369"/>
+      <c r="I5" s="369"/>
+      <c r="J5" s="369"/>
+      <c r="K5" s="369"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="94" t="s">
@@ -52610,12 +52670,12 @@
       <c r="C14" s="98"/>
       <c r="D14" s="98"/>
       <c r="E14" s="98"/>
-      <c r="F14" s="384" t="s">
+      <c r="F14" s="386" t="s">
         <v>262</v>
       </c>
-      <c r="G14" s="384"/>
-      <c r="H14" s="384"/>
-      <c r="I14" s="384"/>
+      <c r="G14" s="386"/>
+      <c r="H14" s="386"/>
+      <c r="I14" s="386"/>
       <c r="J14" s="96"/>
       <c r="K14" s="96"/>
     </row>
@@ -54219,13 +54279,13 @@
     </row>
     <row r="21" spans="1:13" s="160" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="147"/>
-      <c r="B21" s="385" t="s">
+      <c r="B21" s="387" t="s">
         <v>481</v>
       </c>
-      <c r="C21" s="385"/>
-      <c r="D21" s="385"/>
-      <c r="E21" s="385"/>
-      <c r="F21" s="385"/>
+      <c r="C21" s="387"/>
+      <c r="D21" s="387"/>
+      <c r="E21" s="387"/>
+      <c r="F21" s="387"/>
       <c r="G21" s="55"/>
       <c r="H21" s="55"/>
       <c r="I21" s="55"/>
@@ -54425,13 +54485,13 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
       <c r="A33" s="147"/>
-      <c r="B33" s="385" t="s">
+      <c r="B33" s="387" t="s">
         <v>481</v>
       </c>
-      <c r="C33" s="385"/>
-      <c r="D33" s="385"/>
-      <c r="E33" s="385"/>
-      <c r="F33" s="385"/>
+      <c r="C33" s="387"/>
+      <c r="D33" s="387"/>
+      <c r="E33" s="387"/>
+      <c r="F33" s="387"/>
       <c r="H33" s="55"/>
       <c r="I33" s="55"/>
       <c r="J33" s="55"/>
@@ -56736,14 +56796,14 @@
       <c r="G6" s="149"/>
       <c r="H6" s="149"/>
       <c r="I6" s="149"/>
-      <c r="J6" s="386" t="s">
+      <c r="J6" s="388" t="s">
         <v>465</v>
       </c>
-      <c r="K6" s="386"/>
-      <c r="L6" s="386"/>
-      <c r="M6" s="386"/>
-      <c r="N6" s="386"/>
-      <c r="O6" s="386"/>
+      <c r="K6" s="388"/>
+      <c r="L6" s="388"/>
+      <c r="M6" s="388"/>
+      <c r="N6" s="388"/>
+      <c r="O6" s="388"/>
       <c r="P6" s="153"/>
       <c r="Q6" s="153"/>
     </row>
@@ -67733,12 +67793,12 @@
       <c r="C19" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="387" t="s">
+      <c r="G19" s="389" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="387"/>
-      <c r="I19" s="387"/>
-      <c r="J19" s="387"/>
+      <c r="H19" s="389"/>
+      <c r="I19" s="389"/>
+      <c r="J19" s="389"/>
       <c r="L19" s="30" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
Fixed bugs with nested lists. Added P-boxes functionality.
</commit_message>
<xml_diff>
--- a/Current_Financial_Model.xlsx
+++ b/Current_Financial_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Francis/PycharmProjects/VerticalFarming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15217002-06B2-BA41-9954-12948D157AE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ACA535-6D49-7240-92A8-1CBF2685BFBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24400" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24400" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="14" r:id="rId1"/>
@@ -5921,24 +5921,17 @@
     <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5967,9 +5960,16 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6205,7 +6205,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -6335,7 +6335,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -6456,7 +6456,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -6586,7 +6586,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -6707,7 +6707,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -6837,7 +6837,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -6958,7 +6958,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -7088,7 +7088,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.24285589089229545</c:v>
+                  <c:v>0.15605471465192411</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.9592599494643438E-2</c:v>
@@ -7499,7 +7499,7 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-54183.002379510188</c:v>
+                  <c:v>34816.997620489827</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-11064.487365538342</c:v>
@@ -7629,7 +7629,7 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-54183.002379510188</c:v>
+                  <c:v>34816.997620489827</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-11064.487365538342</c:v>
@@ -8459,7 +8459,7 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-54183.002379510188</c:v>
+                  <c:v>34816.997620489827</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-11064.487365538342</c:v>
@@ -8529,7 +8529,7 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>124307.24614000942</c:v>
+                  <c:v>213307.24614000943</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>244160.53625738036</c:v>
@@ -8739,7 +8739,7 @@
                 <c:formatCode>_("£"* #,##0.00_);_("£"* \(#,##0.00\);_("£"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-15546.69029716275</c:v>
+                  <c:v>73453.309702837258</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>37718.008873324041</c:v>
@@ -11526,7 +11526,7 @@
                   <c:v>0.9022472241454822</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.2741379547757472</c:v>
+                  <c:v>-0.12741379547757473</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.0097648469642859</c:v>
@@ -14238,8 +14238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1FB0-CD2F-E14E-8300-C92D3DA9F93F}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView topLeftCell="A105" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -15393,7 +15393,7 @@
       </c>
       <c r="B128">
         <f>target_productivity_CO2_net</f>
-        <v>-100</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -15656,7 +15656,7 @@
       </c>
       <c r="D6" s="49">
         <f>Overview!H81</f>
-        <v>124307.24614000942</v>
+        <v>213307.24614000943</v>
       </c>
       <c r="E6" s="49">
         <f>Overview!I81</f>
@@ -15814,7 +15814,7 @@
       </c>
       <c r="D8" s="50">
         <f>Overview!H92</f>
-        <v>59663.30970283725</v>
+        <v>148663.30970283726</v>
       </c>
       <c r="E8" s="50">
         <f>Overview!I92</f>
@@ -16030,7 +16030,7 @@
       </c>
       <c r="D12" s="50">
         <f>Overview!H102</f>
-        <v>-15546.69029716275</v>
+        <v>73453.309702837258</v>
       </c>
       <c r="E12" s="50">
         <f>Overview!I102</f>
@@ -16395,7 +16395,7 @@
       </c>
       <c r="D18" s="78">
         <f>D12-(D12*Overview!$B$56)-D14-D16</f>
-        <v>-54183.002379510188</v>
+        <v>34816.997620489827</v>
       </c>
       <c r="E18" s="78">
         <f>E12-(E12*Overview!$B$56)-E14-E16</f>
@@ -16471,63 +16471,63 @@
       <c r="C19" s="51"/>
       <c r="D19" s="51">
         <f>-H3+D12</f>
-        <v>-238654.32083654255</v>
+        <v>-149654.32083654255</v>
       </c>
       <c r="E19" s="51">
         <f>D19+E12</f>
-        <v>-200936.3119632185</v>
+        <v>-111936.31196321851</v>
       </c>
       <c r="F19" s="51">
         <f>E19+F12</f>
-        <v>-159834.75659976277</v>
+        <v>-70834.756599762768</v>
       </c>
       <c r="G19" s="51">
         <f t="shared" ref="G19:J19" si="0">F19+G12</f>
-        <v>-116301.27719652497</v>
+        <v>-27301.27719652497</v>
       </c>
       <c r="H19" s="51">
         <f>G19+H12</f>
-        <v>-70526.19824357488</v>
+        <v>18473.80175642512</v>
       </c>
       <c r="I19" s="51">
         <f t="shared" si="0"/>
-        <v>-22699.844230982519</v>
+        <v>66300.155769017481</v>
       </c>
       <c r="J19" s="51">
         <f t="shared" si="0"/>
-        <v>27029.754682308878</v>
+        <v>116029.75468230888</v>
       </c>
       <c r="K19" s="51">
         <f t="shared" ref="K19:R19" si="1">J19+K12</f>
-        <v>78070.477860526371</v>
+        <v>167070.47786052636</v>
       </c>
       <c r="L19" s="51">
         <f t="shared" si="1"/>
-        <v>130337.73664141653</v>
+        <v>219337.7366414165</v>
       </c>
       <c r="M19" s="51">
         <f t="shared" si="1"/>
-        <v>183768.08952828951</v>
+        <v>272768.08952828945</v>
       </c>
       <c r="N19" s="51">
         <f t="shared" si="1"/>
-        <v>238276.94785889192</v>
+        <v>327276.94785889186</v>
       </c>
       <c r="O19" s="51">
         <f t="shared" si="1"/>
-        <v>293800.87013653381</v>
+        <v>382800.87013653375</v>
       </c>
       <c r="P19" s="51">
         <f t="shared" si="1"/>
-        <v>350297.56203008851</v>
+        <v>439297.56203008845</v>
       </c>
       <c r="Q19" s="51">
         <f t="shared" si="1"/>
-        <v>407703.5820428661</v>
+        <v>496703.58204286604</v>
       </c>
       <c r="R19" s="51">
         <f t="shared" si="1"/>
-        <v>465955.4886781766</v>
+        <v>554955.48867817654</v>
       </c>
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
@@ -16608,7 +16608,7 @@
       <c r="C21" s="15"/>
       <c r="D21" s="76">
         <f>(D18/$H$3)</f>
-        <v>-0.24285589089229545</v>
+        <v>0.15605471465192411</v>
       </c>
       <c r="E21" s="76">
         <f t="shared" ref="E21:R21" si="2">(E18/$H$3)</f>
@@ -16710,9 +16710,9 @@
       <c r="B23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="17" t="str">
+      <c r="C23" s="17">
         <f>IF(D19&gt;0,D20,IF(E19&gt;0,E20,IF(F19&gt;0,F20,IF(G19&gt;0,G20,IF(H19&gt;0,H20,"&gt; 5 years")))))</f>
-        <v>&gt; 5 years</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -45302,8 +45302,8 @@
   </sheetPr>
   <dimension ref="A1:V156"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -45322,26 +45322,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="13">
-      <c r="A1" s="368" t="s">
+      <c r="A1" s="381" t="s">
         <v>518</v>
       </c>
-      <c r="B1" s="369"/>
-      <c r="C1" s="369"/>
-      <c r="D1" s="369"/>
-      <c r="E1" s="369"/>
-      <c r="F1" s="369"/>
-      <c r="G1" s="369"/>
-      <c r="H1" s="369"/>
+      <c r="B1" s="382"/>
+      <c r="C1" s="382"/>
+      <c r="D1" s="382"/>
+      <c r="E1" s="382"/>
+      <c r="F1" s="382"/>
+      <c r="G1" s="382"/>
+      <c r="H1" s="382"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A2" s="369"/>
-      <c r="B2" s="369"/>
-      <c r="C2" s="369"/>
-      <c r="D2" s="369"/>
-      <c r="E2" s="369"/>
-      <c r="F2" s="369"/>
-      <c r="G2" s="369"/>
-      <c r="H2" s="369"/>
+      <c r="A2" s="382"/>
+      <c r="B2" s="382"/>
+      <c r="C2" s="382"/>
+      <c r="D2" s="382"/>
+      <c r="E2" s="382"/>
+      <c r="F2" s="382"/>
+      <c r="G2" s="382"/>
+      <c r="H2" s="382"/>
     </row>
     <row r="3" spans="1:22" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="59" t="s">
@@ -45349,28 +45349,28 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="13">
-      <c r="A4" s="370" t="s">
+      <c r="A4" s="383" t="s">
         <v>517</v>
       </c>
-      <c r="B4" s="369"/>
-      <c r="C4" s="369"/>
-      <c r="D4" s="369"/>
-      <c r="E4" s="369"/>
-      <c r="F4" s="369"/>
-      <c r="G4" s="369"/>
-      <c r="H4" s="369"/>
+      <c r="B4" s="382"/>
+      <c r="C4" s="382"/>
+      <c r="D4" s="382"/>
+      <c r="E4" s="382"/>
+      <c r="F4" s="382"/>
+      <c r="G4" s="382"/>
+      <c r="H4" s="382"/>
     </row>
     <row r="5" spans="1:22" ht="13">
-      <c r="A5" s="371" t="s">
+      <c r="A5" s="384" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="369"/>
-      <c r="C5" s="369"/>
-      <c r="D5" s="369"/>
-      <c r="E5" s="369"/>
-      <c r="F5" s="369"/>
-      <c r="G5" s="369"/>
-      <c r="H5" s="369"/>
+      <c r="B5" s="382"/>
+      <c r="C5" s="382"/>
+      <c r="D5" s="382"/>
+      <c r="E5" s="382"/>
+      <c r="F5" s="382"/>
+      <c r="G5" s="382"/>
+      <c r="H5" s="382"/>
     </row>
     <row r="6" spans="1:22" s="26" customFormat="1" ht="13">
       <c r="A6" s="92" t="s">
@@ -45385,16 +45385,16 @@
       <c r="H6" s="93"/>
     </row>
     <row r="7" spans="1:22" ht="13">
-      <c r="A7" s="372" t="s">
+      <c r="A7" s="385" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="369"/>
-      <c r="C7" s="369"/>
-      <c r="D7" s="369"/>
-      <c r="E7" s="369"/>
-      <c r="F7" s="369"/>
-      <c r="G7" s="369"/>
-      <c r="H7" s="369"/>
+      <c r="B7" s="382"/>
+      <c r="C7" s="382"/>
+      <c r="D7" s="382"/>
+      <c r="E7" s="382"/>
+      <c r="F7" s="382"/>
+      <c r="G7" s="382"/>
+      <c r="H7" s="382"/>
     </row>
     <row r="8" spans="1:22" s="26" customFormat="1" ht="13">
       <c r="A8" s="256" t="s">
@@ -45458,8 +45458,8 @@
       <c r="Q13" s="218"/>
       <c r="R13" s="219"/>
       <c r="S13" s="219"/>
-      <c r="T13" s="367"/>
-      <c r="U13" s="367"/>
+      <c r="T13" s="380"/>
+      <c r="U13" s="380"/>
     </row>
     <row r="14" spans="1:22" ht="16">
       <c r="A14" s="2" t="s">
@@ -45644,7 +45644,7 @@
       </c>
       <c r="D18" s="269"/>
       <c r="E18" s="269"/>
-      <c r="F18" s="374" t="s">
+      <c r="F18" s="367" t="s">
         <v>618</v>
       </c>
       <c r="G18" s="323" t="s">
@@ -45695,7 +45695,7 @@
       </c>
       <c r="D19" s="269"/>
       <c r="E19" s="269"/>
-      <c r="F19" s="374"/>
+      <c r="F19" s="367"/>
       <c r="G19" s="292" t="s">
         <v>585</v>
       </c>
@@ -45842,7 +45842,7 @@
       </c>
       <c r="D23" s="269"/>
       <c r="E23" s="269"/>
-      <c r="F23" s="383" t="s">
+      <c r="F23" s="378" t="s">
         <v>316</v>
       </c>
       <c r="G23" s="326" t="s">
@@ -45874,7 +45874,7 @@
       </c>
       <c r="D24" s="269"/>
       <c r="E24" s="269"/>
-      <c r="F24" s="383"/>
+      <c r="F24" s="378"/>
       <c r="G24" s="326" t="s">
         <v>596</v>
       </c>
@@ -45906,7 +45906,7 @@
       </c>
       <c r="D25" s="269"/>
       <c r="E25" s="269"/>
-      <c r="F25" s="382" t="s">
+      <c r="F25" s="377" t="s">
         <v>542</v>
       </c>
       <c r="G25" s="323" t="s">
@@ -45947,7 +45947,7 @@
       </c>
       <c r="D26" s="269"/>
       <c r="E26" s="269"/>
-      <c r="F26" s="382"/>
+      <c r="F26" s="377"/>
       <c r="G26" s="323" t="s">
         <v>315</v>
       </c>
@@ -45976,7 +45976,7 @@
       <c r="A27" s="4"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
-      <c r="F27" s="380" t="s">
+      <c r="F27" s="375" t="s">
         <v>588</v>
       </c>
       <c r="G27" s="185" t="s">
@@ -46009,7 +46009,7 @@
       </c>
       <c r="B28" s="54"/>
       <c r="C28" s="47"/>
-      <c r="F28" s="381"/>
+      <c r="F28" s="376"/>
       <c r="G28" s="185" t="s">
         <v>315</v>
       </c>
@@ -46042,7 +46042,7 @@
         <v>79</v>
       </c>
       <c r="C29" s="47"/>
-      <c r="F29" s="384" t="s">
+      <c r="F29" s="379" t="s">
         <v>587</v>
       </c>
       <c r="G29" s="185" t="s">
@@ -46077,7 +46077,7 @@
         <v>865</v>
       </c>
       <c r="C30" s="170"/>
-      <c r="F30" s="381"/>
+      <c r="F30" s="376"/>
       <c r="G30" s="185" t="s">
         <v>483</v>
       </c>
@@ -46110,7 +46110,7 @@
         <v>165</v>
       </c>
       <c r="C31" s="170"/>
-      <c r="F31" s="376" t="s">
+      <c r="F31" s="371" t="s">
         <v>531</v>
       </c>
       <c r="G31" s="212" t="s">
@@ -46142,7 +46142,7 @@
         <v>164</v>
       </c>
       <c r="C32" s="170"/>
-      <c r="F32" s="377"/>
+      <c r="F32" s="372"/>
       <c r="G32" s="212" t="s">
         <v>315</v>
       </c>
@@ -46201,7 +46201,7 @@
       <c r="B34" s="356" t="s">
         <v>165</v>
       </c>
-      <c r="F34" s="373" t="s">
+      <c r="F34" s="370" t="s">
         <v>615</v>
       </c>
       <c r="G34" s="185" t="s">
@@ -46235,7 +46235,7 @@
       <c r="C35" s="254" t="s">
         <v>489</v>
       </c>
-      <c r="F35" s="373"/>
+      <c r="F35" s="370"/>
       <c r="G35" s="185" t="s">
         <v>533</v>
       </c>
@@ -46267,7 +46267,7 @@
       <c r="C36" s="264">
         <v>8</v>
       </c>
-      <c r="F36" s="373"/>
+      <c r="F36" s="370"/>
       <c r="G36" s="185" t="s">
         <v>534</v>
       </c>
@@ -46300,7 +46300,7 @@
         <f>C36*16</f>
         <v>128</v>
       </c>
-      <c r="F37" s="373"/>
+      <c r="F37" s="370"/>
       <c r="G37" s="185" t="s">
         <v>535</v>
       </c>
@@ -46331,7 +46331,7 @@
         <f>C36*VLOOKUP(B36, Database!A97:I107, 5, FALSE)</f>
         <v>2880</v>
       </c>
-      <c r="F38" s="373"/>
+      <c r="F38" s="370"/>
       <c r="G38" s="185" t="s">
         <v>536</v>
       </c>
@@ -46361,7 +46361,7 @@
         <v>507</v>
       </c>
       <c r="C39" s="170"/>
-      <c r="F39" s="378" t="s">
+      <c r="F39" s="373" t="s">
         <v>589</v>
       </c>
       <c r="G39" s="212" t="s">
@@ -46393,7 +46393,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="170"/>
-      <c r="F40" s="379"/>
+      <c r="F40" s="374"/>
       <c r="G40" s="212" t="s">
         <v>315</v>
       </c>
@@ -46427,7 +46427,7 @@
       </c>
       <c r="C41" s="170"/>
       <c r="D41" s="55"/>
-      <c r="F41" s="374" t="s">
+      <c r="F41" s="367" t="s">
         <v>613</v>
       </c>
       <c r="G41" s="292" t="s">
@@ -46458,7 +46458,7 @@
         <v>166</v>
       </c>
       <c r="C42" s="170"/>
-      <c r="F42" s="374"/>
+      <c r="F42" s="367"/>
       <c r="G42" s="212" t="s">
         <v>614</v>
       </c>
@@ -46496,11 +46496,11 @@
         <v>722</v>
       </c>
       <c r="C44" s="170"/>
-      <c r="G44" s="385" t="s">
+      <c r="G44" s="369" t="s">
         <v>602</v>
       </c>
-      <c r="H44" s="385"/>
-      <c r="I44" s="385"/>
+      <c r="H44" s="369"/>
+      <c r="I44" s="369"/>
     </row>
     <row r="45" spans="1:12" s="160" customFormat="1" ht="16">
       <c r="A45" s="171" t="s">
@@ -46807,11 +46807,11 @@
         <v>127.41379547757472</v>
       </c>
       <c r="J54" s="275">
-        <v>-100</v>
+        <v>-1000</v>
       </c>
       <c r="K54" s="183">
-        <f t="shared" si="2"/>
-        <v>-1.2741379547757472</v>
+        <f>I54/J54</f>
+        <v>-0.12741379547757473</v>
       </c>
       <c r="L54" s="269">
         <v>1</v>
@@ -47935,7 +47935,7 @@
         <v>102</v>
       </c>
       <c r="H80" s="261">
-        <v>0</v>
+        <v>89000</v>
       </c>
       <c r="I80" s="260"/>
       <c r="J80" s="262" t="s">
@@ -47996,7 +47996,7 @@
       </c>
       <c r="H81" s="38">
         <f>SUM(H75:H80)</f>
-        <v>124307.24614000942</v>
+        <v>213307.24614000943</v>
       </c>
       <c r="I81" s="38">
         <f>SUM(I75:I80)</f>
@@ -48732,7 +48732,7 @@
       </c>
       <c r="H92" s="83">
         <f>H81-H90</f>
-        <v>59663.30970283725</v>
+        <v>148663.30970283726</v>
       </c>
       <c r="I92" s="83">
         <f t="shared" ref="I92:V92" si="13">I81-I90</f>
@@ -49382,7 +49382,7 @@
       </c>
       <c r="H102" s="43">
         <f>H92-H100</f>
-        <v>-15546.69029716275</v>
+        <v>73453.309702837258</v>
       </c>
       <c r="I102" s="43">
         <f>I92-I100</f>
@@ -49809,7 +49809,7 @@
       </c>
       <c r="H109" s="42">
         <f>H102-H106-H104-H107</f>
-        <v>-54183.002379510188</v>
+        <v>34816.997620489827</v>
       </c>
       <c r="I109" s="42">
         <f t="shared" ref="I109:V109" si="22">I102-I106-I104-I107</f>
@@ -51878,17 +51878,17 @@
     </row>
     <row r="142" spans="1:22" ht="15.75" customHeight="1">
       <c r="F142" s="269"/>
-      <c r="G142" s="374" t="s">
+      <c r="G142" s="367" t="s">
         <v>632</v>
       </c>
-      <c r="H142" s="375"/>
-      <c r="I142" s="375"/>
+      <c r="H142" s="368"/>
+      <c r="I142" s="368"/>
       <c r="K142" s="269"/>
-      <c r="L142" s="374" t="s">
+      <c r="L142" s="367" t="s">
         <v>633</v>
       </c>
-      <c r="M142" s="375"/>
-      <c r="N142" s="375"/>
+      <c r="M142" s="368"/>
+      <c r="N142" s="368"/>
     </row>
     <row r="143" spans="1:22" ht="15.75" customHeight="1">
       <c r="F143" s="272" t="s">
@@ -52227,17 +52227,17 @@
     </row>
     <row r="153" spans="6:17" ht="15.75" customHeight="1">
       <c r="F153" s="269"/>
-      <c r="G153" s="374" t="s">
+      <c r="G153" s="367" t="s">
         <v>631</v>
       </c>
-      <c r="H153" s="374"/>
-      <c r="I153" s="374"/>
+      <c r="H153" s="367"/>
+      <c r="I153" s="367"/>
       <c r="K153" s="269"/>
-      <c r="L153" s="374" t="s">
+      <c r="L153" s="367" t="s">
         <v>631</v>
       </c>
-      <c r="M153" s="374"/>
-      <c r="N153" s="374"/>
+      <c r="M153" s="367"/>
+      <c r="N153" s="367"/>
       <c r="P153" s="47" t="s">
         <v>64</v>
       </c>
@@ -52344,11 +52344,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G153:I153"/>
-    <mergeCell ref="L142:N142"/>
-    <mergeCell ref="L153:N153"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="F34:F38"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="G142:I142"/>
@@ -52358,11 +52358,11 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="F29:F30"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="G153:I153"/>
+    <mergeCell ref="L142:N142"/>
+    <mergeCell ref="L153:N153"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="F41:F42"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="L16">
@@ -52474,8 +52474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1AB830-BB86-434F-80B6-DAC5753A91A4}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="89" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="A49" zoomScale="92" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -52504,34 +52504,34 @@
       <c r="K1" s="96"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="370" t="s">
+      <c r="A2" s="383" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="370"/>
-      <c r="C2" s="369"/>
-      <c r="D2" s="369"/>
-      <c r="E2" s="369"/>
-      <c r="F2" s="369"/>
-      <c r="G2" s="369"/>
-      <c r="H2" s="369"/>
-      <c r="I2" s="369"/>
-      <c r="J2" s="369"/>
-      <c r="K2" s="369"/>
+      <c r="B2" s="383"/>
+      <c r="C2" s="382"/>
+      <c r="D2" s="382"/>
+      <c r="E2" s="382"/>
+      <c r="F2" s="382"/>
+      <c r="G2" s="382"/>
+      <c r="H2" s="382"/>
+      <c r="I2" s="382"/>
+      <c r="J2" s="382"/>
+      <c r="K2" s="382"/>
     </row>
     <row r="3" spans="1:11" s="96" customFormat="1">
-      <c r="A3" s="371" t="s">
+      <c r="A3" s="384" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="371"/>
-      <c r="C3" s="369"/>
-      <c r="D3" s="369"/>
-      <c r="E3" s="369"/>
-      <c r="F3" s="369"/>
-      <c r="G3" s="369"/>
-      <c r="H3" s="369"/>
-      <c r="I3" s="369"/>
-      <c r="J3" s="369"/>
-      <c r="K3" s="369"/>
+      <c r="B3" s="384"/>
+      <c r="C3" s="382"/>
+      <c r="D3" s="382"/>
+      <c r="E3" s="382"/>
+      <c r="F3" s="382"/>
+      <c r="G3" s="382"/>
+      <c r="H3" s="382"/>
+      <c r="I3" s="382"/>
+      <c r="J3" s="382"/>
+      <c r="K3" s="382"/>
     </row>
     <row r="4" spans="1:11" s="96" customFormat="1">
       <c r="A4" s="92" t="s">
@@ -52549,19 +52549,19 @@
       <c r="K4" s="93"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="372" t="s">
+      <c r="A5" s="385" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="372"/>
-      <c r="C5" s="369"/>
-      <c r="D5" s="369"/>
-      <c r="E5" s="369"/>
-      <c r="F5" s="369"/>
-      <c r="G5" s="369"/>
-      <c r="H5" s="369"/>
-      <c r="I5" s="369"/>
-      <c r="J5" s="369"/>
-      <c r="K5" s="369"/>
+      <c r="B5" s="385"/>
+      <c r="C5" s="382"/>
+      <c r="D5" s="382"/>
+      <c r="E5" s="382"/>
+      <c r="F5" s="382"/>
+      <c r="G5" s="382"/>
+      <c r="H5" s="382"/>
+      <c r="I5" s="382"/>
+      <c r="J5" s="382"/>
+      <c r="K5" s="382"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="94" t="s">
@@ -53795,6 +53795,7 @@
     <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -56678,9 +56679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D044E3B-C1AC-D346-B4EB-4AAE890C9158}">
   <dimension ref="A1:AA199"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" zoomScale="99" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A96" sqref="A96:I107"/>
+    <sheetView topLeftCell="A18" zoomScale="99" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>